<commit_message>
LCA completed, visualization in progress
</commit_message>
<xml_diff>
--- a/data/LCA.xlsx
+++ b/data/LCA.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnergyDevelopment_Policy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68823686-5EB9-4E62-9116-CF2009EB3821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D6674A-6F38-48EE-9B5C-87D7AD3F5799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4650" windowWidth="29040" windowHeight="15840" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="CCGT" sheetId="1" r:id="rId1"/>
+    <sheet name="LCA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Table 1: CCGT Life Cycle Analysis Emissions Rate</t>
   </si>
@@ -98,9 +98,6 @@
       </rPr>
       <t>x</t>
     </r>
-  </si>
-  <si>
-    <t>(lb/MWh)</t>
   </si>
   <si>
     <r>
@@ -185,14 +182,123 @@
     <t>Table 2: CCGT Life Cycle Analysis Annual Emissions</t>
   </si>
   <si>
-    <t>(lb/year)</t>
+    <t>(gal/MWh)</t>
+  </si>
+  <si>
+    <t>Slide 23</t>
+  </si>
+  <si>
+    <t>slide 24</t>
+  </si>
+  <si>
+    <t>Water Consumption*</t>
+  </si>
+  <si>
+    <t>Water Withdrawl*</t>
+  </si>
+  <si>
+    <t>* Assumed recirculating cooling (cooling towers)</t>
+  </si>
+  <si>
+    <t>(10^6 gal/year)</t>
+  </si>
+  <si>
+    <t>Table 3: CCGT Life Cycle Analysis Water Consumption and Withdrawl [3]</t>
+  </si>
+  <si>
+    <t>Big Sky</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>(MW)</t>
+  </si>
+  <si>
+    <t>XIT Ranch</t>
+  </si>
+  <si>
+    <t>Onshore Wind</t>
+  </si>
+  <si>
+    <t>Project Area</t>
+  </si>
+  <si>
+    <t>(acres)</t>
+  </si>
+  <si>
+    <t>Season Factors</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Non-Summer</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Rest of Year</t>
+  </si>
+  <si>
+    <t>Summer Peak</t>
+  </si>
+  <si>
+    <t>Summer Off-peak</t>
+  </si>
+  <si>
+    <t>WTC</t>
+  </si>
+  <si>
+    <t>Lavaca</t>
+  </si>
+  <si>
+    <t>Coastal Wind</t>
+  </si>
+  <si>
+    <t>CO2-eq</t>
+  </si>
+  <si>
+    <t>(g CO2 eq/ kWh)</t>
+  </si>
+  <si>
+    <t>slide 38/ 39</t>
+  </si>
+  <si>
+    <t>(kg CO2 eq/year)</t>
+  </si>
+  <si>
+    <t>Table 4: Renewables Life Cycle Analysis [4]</t>
+  </si>
+  <si>
+    <t>(s.t./year)</t>
+  </si>
+  <si>
+    <t>(lb/MMBtu)</t>
+  </si>
+  <si>
+    <t>0.15 / 0.0075</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +339,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -242,7 +354,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -333,11 +445,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -357,6 +630,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -372,8 +648,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,350 +1020,764 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27891372-5872-4E4D-8E46-0ACC3C9C1CC7}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="B1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:Q7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
-      <c r="J1" s="7" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="K2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="10"/>
+    </row>
+    <row r="3" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="E5" s="5">
+        <v>6800</v>
+      </c>
+      <c r="F5" s="5">
+        <v>600</v>
+      </c>
+      <c r="G5" s="5">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="I5" s="5">
+        <v>117</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="N5" s="5">
+        <v>6800</v>
+      </c>
+      <c r="O5" s="5">
+        <v>600</v>
+      </c>
+      <c r="P5" s="7">
+        <f>$D5*8760*$F5*G5/2000</f>
+        <v>5.2625699999999993</v>
+      </c>
+      <c r="Q5" s="7">
+        <f>$D5*8760*$F5*H5/2000</f>
+        <v>0.51924024000000002</v>
+      </c>
+      <c r="R5" s="7">
+        <f>$D5*8760*$F5*I5/2000</f>
+        <v>82096.092000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.314</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6400</v>
+      </c>
+      <c r="F6" s="5">
+        <v>460</v>
+      </c>
+      <c r="G6" s="5">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="I6" s="5">
+        <v>117</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.314</v>
+      </c>
+      <c r="N6" s="5">
+        <v>6400</v>
+      </c>
+      <c r="O6" s="5">
+        <v>460</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" ref="P6:P8" si="0">$D6*8760*$F6*G6/2000</f>
+        <v>4.7448539999999992</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" ref="Q6:Q8" si="1">$D6*8760*$F6*H6/2000</f>
+        <v>0.46815892799999992</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" ref="R6:R8" si="2">$D6*8760*$F6*I6/2000</f>
+        <v>74019.722399999984</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6200</v>
+      </c>
+      <c r="F7" s="5">
+        <v>405</v>
+      </c>
+      <c r="G7" s="5">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H7" s="5">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="I7" s="5">
+        <v>117</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="N7" s="5">
+        <v>6200</v>
+      </c>
+      <c r="O7" s="5">
+        <v>405</v>
+      </c>
+      <c r="P7" s="7">
+        <f t="shared" si="0"/>
+        <v>4.5766619999999998</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.45156398399999997</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="2"/>
+        <v>71395.927200000006</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5">
+        <v>942</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="I8" s="5">
+        <v>117</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="5">
+        <v>942</v>
+      </c>
+      <c r="P8" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32058709199999996</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="2"/>
+        <v>50687.418600000005</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="2:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="Q13" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="R13" s="34"/>
+    </row>
+    <row r="14" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="G14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="37"/>
+      <c r="L14" s="38"/>
+      <c r="Q14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="R14" s="30">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="E15" s="5">
+        <v>600</v>
+      </c>
+      <c r="F15" s="5">
+        <v>200</v>
+      </c>
+      <c r="G15" s="7">
+        <f>$D15*8760*$E15*F15/10^6</f>
+        <v>280.67039999999997</v>
+      </c>
+      <c r="H15" s="5">
+        <v>250</v>
+      </c>
+      <c r="I15" s="7">
+        <f>$D15*8760*$E15*H15/10^6</f>
+        <v>350.83800000000002</v>
+      </c>
+      <c r="Q15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="32">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.314</v>
+      </c>
+      <c r="E16" s="5">
+        <v>460</v>
+      </c>
+      <c r="F16" s="5">
+        <v>200</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" ref="G16:G18" si="3">$D16*8760*$E16*F16/10^6</f>
+        <v>253.05887999999996</v>
+      </c>
+      <c r="H16" s="5">
+        <v>250</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" ref="I16:I18" si="4">$D16*8760*$E16*H16/10^6</f>
+        <v>316.3236</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E17" s="5">
+        <v>405</v>
+      </c>
+      <c r="F17" s="5">
+        <v>200</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="3"/>
+        <v>244.08864</v>
+      </c>
+      <c r="H17" s="5">
+        <v>250</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="4"/>
+        <v>305.11079999999998</v>
+      </c>
+      <c r="Q17" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="34"/>
+    </row>
+    <row r="18" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="E18" s="5">
+        <v>942</v>
+      </c>
+      <c r="F18" s="5">
+        <v>200</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="3"/>
+        <v>173.29032000000001</v>
+      </c>
+      <c r="H18" s="5">
+        <v>250</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="4"/>
+        <v>216.6129</v>
+      </c>
+      <c r="Q18" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="R18" s="30">
+        <f>R15*(22/24)</f>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17"/>
+      <c r="Q19" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="R19" s="30">
+        <f>R14-R20</f>
+        <v>0.16666666666666669</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q20" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="R20" s="30">
+        <f>R14*(8/24)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="R21" s="32">
+        <f>R15-R18</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="23"/>
+    </row>
+    <row r="23" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="D4" s="5">
-        <v>6800</v>
-      </c>
-      <c r="E4" s="5">
-        <v>600</v>
-      </c>
-      <c r="F4" s="5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G4" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H4" s="5">
-        <v>821.096</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="M4" s="5">
-        <v>6800</v>
-      </c>
-      <c r="N4" s="5">
-        <v>600</v>
-      </c>
-      <c r="O4" s="12">
-        <f>$C4*8670*$E4*F4/2000</f>
-        <v>52.779492000000005</v>
-      </c>
-      <c r="P4" s="12">
-        <f t="shared" ref="P4:Q7" si="0">$C4*8670*$E4*G4/2000</f>
-        <v>2.7778680000000002</v>
-      </c>
-      <c r="Q4" s="12">
-        <f t="shared" si="0"/>
-        <v>570224.07583200012</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="E23" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="35">
+        <f>R15*0.203+R14*0.702</f>
+        <v>0.32774999999999999</v>
+      </c>
+      <c r="E25" s="19">
+        <v>250</v>
+      </c>
+      <c r="F25" s="19">
+        <v>8000</v>
+      </c>
+      <c r="G25" s="19">
+        <v>55</v>
+      </c>
+      <c r="H25" s="20">
+        <f>D25*E25*8760*G25/(10^6)</f>
+        <v>39.477487500000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="35">
+        <f>0.53*R18+0.342*R19+0.49*R20+0.53*R21</f>
+        <v>0.49533333333333335</v>
+      </c>
+      <c r="E26" s="19">
+        <v>250</v>
+      </c>
+      <c r="F26" s="19">
+        <v>38000</v>
+      </c>
+      <c r="G26" s="19">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0.314</v>
-      </c>
-      <c r="D5" s="5">
-        <v>6400</v>
-      </c>
-      <c r="E5" s="5">
-        <v>460</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="G5" s="5">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1377.1759999999999</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="H26" s="20">
+        <f t="shared" ref="H26:H28" si="5">D26*E26*8760*G26/(10^6)</f>
+        <v>14.10214</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="35">
+        <f>0.498*R15+0.435*R19+0.456*R20</f>
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="E27" s="19">
+        <v>200</v>
+      </c>
+      <c r="F27" s="19">
+        <v>20000</v>
+      </c>
+      <c r="G27" s="19">
         <v>13</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0.314</v>
-      </c>
-      <c r="M5" s="5">
-        <v>6400</v>
-      </c>
-      <c r="N5" s="5">
-        <v>460</v>
-      </c>
-      <c r="O5" s="12">
-        <f t="shared" ref="O5:O7" si="1">$C5*8670*$E5*F5/2000</f>
-        <v>526.58996339999999</v>
-      </c>
-      <c r="P5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.3830318000000004</v>
-      </c>
-      <c r="Q5" s="12">
-        <f t="shared" si="0"/>
-        <v>862315.17174239992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="D6" s="5">
-        <v>6200</v>
-      </c>
-      <c r="E6" s="5">
-        <v>405</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.499</v>
-      </c>
-      <c r="G6" s="5">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1465.011</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="M6" s="5">
-        <v>6200</v>
-      </c>
-      <c r="N6" s="5">
-        <v>405</v>
-      </c>
-      <c r="O6" s="12">
-        <f t="shared" si="1"/>
-        <v>301.37214779999999</v>
-      </c>
-      <c r="P6" s="12">
-        <f t="shared" si="0"/>
-        <v>4.2276654000000002</v>
-      </c>
-      <c r="Q6" s="12">
-        <f t="shared" si="0"/>
-        <v>884796.61647419992</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.105</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5">
-        <v>942</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.115</v>
-      </c>
-      <c r="G7" s="5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H7" s="5">
-        <v>914.01400000000001</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0.105</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="5">
-        <v>942</v>
-      </c>
-      <c r="O7" s="12">
-        <f t="shared" si="1"/>
-        <v>49.309107750000003</v>
-      </c>
-      <c r="P7" s="12">
-        <f t="shared" si="0"/>
-        <v>2.1438742500000001</v>
-      </c>
-      <c r="Q7" s="12">
-        <f t="shared" si="0"/>
-        <v>391906.21574790002</v>
+      <c r="H27" s="20">
+        <f t="shared" si="5"/>
+        <v>11.023584</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="35">
+        <f>0.454*R15+0.419*R19+0.428*R20</f>
+        <v>0.44600000000000006</v>
+      </c>
+      <c r="E28" s="19">
+        <v>150</v>
+      </c>
+      <c r="F28" s="19">
+        <v>20000</v>
+      </c>
+      <c r="G28" s="19">
+        <v>13</v>
+      </c>
+      <c r="H28" s="20">
+        <f t="shared" si="5"/>
+        <v>7.6185720000000003</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
+  <mergeCells count="24">
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mid-semester memo updates, mostly visualization
</commit_message>
<xml_diff>
--- a/data/LCA.xlsx
+++ b/data/LCA.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnergyDevelopment_Policy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D6674A-6F38-48EE-9B5C-87D7AD3F5799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C77D6C-D1B4-40A7-9061-85EB044E2E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
+    <sheet name="Capacity Factors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t>Table 1: CCGT Life Cycle Analysis Emissions Rate</t>
   </si>
@@ -287,7 +288,7 @@
     <t>(lb/MMBtu)</t>
   </si>
   <si>
-    <t>0.15 / 0.0075</t>
+    <t>Raw CF</t>
   </si>
 </sst>
 </file>
@@ -295,8 +296,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -633,77 +634,77 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27891372-5872-4E4D-8E46-0ACC3C9C1CC7}">
-  <dimension ref="B1:R28"/>
+  <dimension ref="B1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B5" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,41 +1041,41 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="K2" s="8" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="K2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="34"/>
     </row>
     <row r="3" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="35" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1086,19 +1087,19 @@
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="35" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="35" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -1112,13 +1113,13 @@
       </c>
     </row>
     <row r="4" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
       <c r="G4" s="3" t="s">
         <v>52</v>
       </c>
@@ -1128,13 +1129,13 @@
       <c r="I4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
       <c r="M4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
       <c r="P4" s="3" t="s">
         <v>51</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>460</v>
       </c>
       <c r="P6" s="7">
-        <f t="shared" ref="P6:P8" si="0">$D6*8760*$F6*G6/2000</f>
+        <f t="shared" ref="P6:P7" si="0">$D6*8760*$F6*G6/2000</f>
         <v>4.7448539999999992</v>
       </c>
       <c r="Q6" s="7">
@@ -1314,14 +1315,14 @@
       <c r="D8" s="6">
         <v>0.105</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>16</v>
+      <c r="E8" s="8">
+        <v>8840</v>
       </c>
       <c r="F8" s="5">
         <v>942</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>53</v>
+      <c r="G8" s="8">
+        <v>0.15</v>
       </c>
       <c r="H8" s="5">
         <v>7.3999999999999999E-4</v>
@@ -1338,15 +1339,15 @@
       <c r="M8" s="6">
         <v>0.105</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="8" t="s">
         <v>16</v>
       </c>
       <c r="O8" s="5">
         <v>942</v>
       </c>
-      <c r="P8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="P8" s="7">
+        <f>$D8*8760*$F8*G8/2000</f>
+        <v>64.983869999999996</v>
       </c>
       <c r="Q8" s="7">
         <f t="shared" si="1"/>
@@ -1357,427 +1358,528 @@
         <v>50687.418600000005</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" t="s">
+    <row r="9" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="E9" s="8">
+        <v>8840</v>
+      </c>
+      <c r="F9" s="5">
+        <v>942</v>
+      </c>
+      <c r="G9" s="8">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="I9" s="5">
+        <v>117</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="5">
+        <v>942</v>
+      </c>
+      <c r="P9" s="7">
+        <f>$D9*8760*$F9*G9/2000</f>
+        <v>3.2491935000000001</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" ref="Q9" si="3">$D9*8760*$F9*H9/2000</f>
+        <v>0.32058709199999996</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" ref="R9" si="4">$D9*8760*$F9*I9/2000</f>
+        <v>50687.418600000005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
+    <row r="13" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="K12" s="36"/>
-    </row>
-    <row r="13" spans="2:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="2:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C14" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="13" t="s">
+      <c r="G14" s="38"/>
+      <c r="H14" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="Q13" s="33" t="s">
+      <c r="I14" s="38"/>
+      <c r="Q14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="R13" s="34"/>
-    </row>
-    <row r="14" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="2" t="s">
+      <c r="R14" s="21"/>
+    </row>
+    <row r="15" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="3" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38"/>
-      <c r="Q14" s="29" t="s">
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
+      <c r="Q15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="30">
+      <c r="R15" s="13">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="E15" s="5">
-        <v>600</v>
-      </c>
-      <c r="F15" s="5">
-        <v>200</v>
-      </c>
-      <c r="G15" s="7">
-        <f>$D15*8760*$E15*F15/10^6</f>
-        <v>280.67039999999997</v>
-      </c>
-      <c r="H15" s="5">
-        <v>250</v>
-      </c>
-      <c r="I15" s="7">
-        <f>$D15*8760*$E15*H15/10^6</f>
-        <v>350.83800000000002</v>
-      </c>
-      <c r="Q15" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="R15" s="32">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="6">
-        <v>0.314</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="E16" s="5">
-        <v>460</v>
+        <v>600</v>
       </c>
       <c r="F16" s="5">
         <v>200</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" ref="G16:G18" si="3">$D16*8760*$E16*F16/10^6</f>
-        <v>253.05887999999996</v>
+        <f>$D16*8760*$E16*F16/10^6</f>
+        <v>280.67039999999997</v>
       </c>
       <c r="H16" s="5">
         <v>250</v>
       </c>
       <c r="I16" s="7">
-        <f t="shared" ref="I16:I18" si="4">$D16*8760*$E16*H16/10^6</f>
-        <v>316.3236</v>
+        <f>$D16*8760*$E16*H16/10^6</f>
+        <v>350.83800000000002</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R16" s="15">
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="6">
-        <v>0.34399999999999997</v>
+        <v>0.314</v>
       </c>
       <c r="E17" s="5">
-        <v>405</v>
+        <v>460</v>
       </c>
       <c r="F17" s="5">
         <v>200</v>
       </c>
       <c r="G17" s="7">
-        <f t="shared" si="3"/>
-        <v>244.08864</v>
+        <f t="shared" ref="G17:G19" si="5">$D17*8760*$E17*F17/10^6</f>
+        <v>253.05887999999996</v>
       </c>
       <c r="H17" s="5">
         <v>250</v>
       </c>
       <c r="I17" s="7">
-        <f t="shared" si="4"/>
-        <v>305.11079999999998</v>
-      </c>
-      <c r="Q17" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="R17" s="34"/>
+        <f t="shared" ref="I17:I19" si="6">$D17*8760*$E17*H17/10^6</f>
+        <v>316.3236</v>
+      </c>
     </row>
     <row r="18" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D18" s="6">
-        <v>0.105</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="E18" s="5">
-        <v>942</v>
+        <v>405</v>
       </c>
       <c r="F18" s="5">
         <v>200</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="3"/>
-        <v>173.29032000000001</v>
+        <f t="shared" si="5"/>
+        <v>244.08864</v>
       </c>
       <c r="H18" s="5">
         <v>250</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
+        <v>305.11079999999998</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="21"/>
+    </row>
+    <row r="19" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="E19" s="5">
+        <v>942</v>
+      </c>
+      <c r="F19" s="5">
+        <v>200</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="5"/>
+        <v>173.29032000000001</v>
+      </c>
+      <c r="H19" s="5">
+        <v>250</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="6"/>
         <v>216.6129</v>
       </c>
-      <c r="Q18" s="29" t="s">
+      <c r="Q19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="R18" s="30">
-        <f>R15*(22/24)</f>
+      <c r="R19" s="13">
+        <f>R16*(22/24)</f>
         <v>0.6875</v>
       </c>
     </row>
-    <row r="19" spans="2:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
+    <row r="20" spans="2:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
-      <c r="Q19" s="29" t="s">
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="Q20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="R19" s="30">
-        <f>R14-R20</f>
+      <c r="R20" s="13">
+        <f>R15-R21</f>
         <v>0.16666666666666669</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="Q20" s="29" t="s">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="R20" s="30">
-        <f>R14*(8/24)</f>
+      <c r="R21" s="13">
+        <f>R15*(8/24)</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G21" t="s">
+    <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
         <v>48</v>
       </c>
-      <c r="Q21" s="31" t="s">
+      <c r="Q22" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="R21" s="32">
-        <f>R15-R18</f>
+      <c r="R22" s="15">
+        <f>R16-R19</f>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+    <row r="23" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-    </row>
-    <row r="23" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
+    </row>
+    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D24" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G24" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="27"/>
-    </row>
-    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="25" t="s">
+      <c r="H24" s="28"/>
+    </row>
+    <row r="25" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H25" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
+    <row r="26" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="35">
-        <f>R15*0.203+R14*0.702</f>
+      <c r="D26" s="16">
+        <f>R16*0.203+R15*0.702</f>
         <v>0.32774999999999999</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E26" s="9">
         <v>250</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F26" s="9">
         <v>8000</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G26" s="9">
         <v>55</v>
       </c>
-      <c r="H25" s="20">
-        <f>D25*E25*8760*G25/(10^6)</f>
+      <c r="H26" s="10">
+        <f>D26*E26*8760*G26/(10^6)</f>
         <v>39.477487500000002</v>
       </c>
     </row>
-    <row r="26" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="19" t="s">
+    <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="35">
-        <f>0.53*R18+0.342*R19+0.49*R20+0.53*R21</f>
+      <c r="D27" s="16">
+        <f>0.53*R19+0.342*R20+0.49*R21+0.53*R22</f>
         <v>0.49533333333333335</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E27" s="9">
         <v>250</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F27" s="9">
         <v>38000</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G27" s="9">
         <v>13</v>
       </c>
-      <c r="H26" s="20">
-        <f t="shared" ref="H26:H28" si="5">D26*E26*8760*G26/(10^6)</f>
+      <c r="H27" s="10">
+        <f t="shared" ref="H27:H29" si="7">D27*E27*8760*G27/(10^6)</f>
         <v>14.10214</v>
       </c>
     </row>
-    <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="19" t="s">
+    <row r="28" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="35">
-        <f>0.498*R15+0.435*R19+0.456*R20</f>
+      <c r="D28" s="16">
+        <f>0.498*R16+0.435*R20+0.456*R21</f>
         <v>0.48399999999999999</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E28" s="9">
         <v>200</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F28" s="9">
         <v>20000</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G28" s="9">
         <v>13</v>
       </c>
-      <c r="H27" s="20">
-        <f t="shared" si="5"/>
+      <c r="H28" s="10">
+        <f t="shared" si="7"/>
         <v>11.023584</v>
       </c>
     </row>
-    <row r="28" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
+    <row r="29" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="35">
-        <f>0.454*R15+0.419*R19+0.428*R20</f>
+      <c r="D29" s="16">
+        <f>0.454*R16+0.419*R20+0.428*R21</f>
         <v>0.44600000000000006</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E29" s="9">
         <v>150</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F29" s="9">
         <v>20000</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G29" s="9">
         <v>13</v>
       </c>
-      <c r="H28" s="20">
-        <f t="shared" si="5"/>
+      <c r="H29" s="10">
+        <f t="shared" si="7"/>
         <v>7.6185720000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="K2:R2"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5564981C-E4C1-4223-BBB8-B7B238FE5FB5}">
+  <dimension ref="B2:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fudge factor for LCA. Pushing before I delete old LCA
</commit_message>
<xml_diff>
--- a/data/LCA.xlsx
+++ b/data/LCA.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnergyDevelopment_Policy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE956B75-B35B-495E-A357-216F5AEAA028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11BEA37-F380-4C61-B4DF-B1BD630C8CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
+    <workbookView xWindow="20370" yWindow="-4650" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
-    <sheet name="LCA_Daily" sheetId="4" r:id="rId2"/>
-    <sheet name="LCA_Hourly" sheetId="6" r:id="rId3"/>
+    <sheet name="LCA_Hourly" sheetId="6" r:id="rId2"/>
+    <sheet name="CF Adjustment" sheetId="2" r:id="rId3"/>
     <sheet name="Marginal Costs" sheetId="5" r:id="rId4"/>
-    <sheet name="CF Adjustment" sheetId="2" r:id="rId5"/>
-    <sheet name="Graphing" sheetId="3" r:id="rId6"/>
+    <sheet name="Graphing" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Graphing!$A$2:$N$424</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Graphing!$A$2:$N$424</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="89">
   <si>
     <t>Table 1: CCGT Life Cycle Analysis Emissions Rate</t>
   </si>
@@ -393,16 +392,26 @@
   <si>
     <t>NG_Price</t>
   </si>
+  <si>
+    <t>Raw CF Daily</t>
+  </si>
+  <si>
+    <t>Raw CF Hourly</t>
+  </si>
+  <si>
+    <t>Adjusted Heat Rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="168" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="177" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,12 +477,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -769,7 +772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -874,9 +877,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -951,12 +951,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6139,8 +6150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27891372-5872-4E4D-8E46-0ACC3C9C1CC7}">
   <dimension ref="B1:S29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I9"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6159,33 +6170,33 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
-      <c r="L2" s="50" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
+      <c r="L2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="52"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="51"/>
     </row>
     <row r="3" spans="2:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -6194,10 +6205,10 @@
       <c r="E3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="52" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -6209,19 +6220,19 @@
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="53" t="s">
+      <c r="L3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="52" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="53" t="s">
+      <c r="O3" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="53" t="s">
+      <c r="P3" s="52" t="s">
         <v>6</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -6235,16 +6246,16 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="3" t="s">
         <v>52</v>
       </c>
@@ -6254,13 +6265,13 @@
       <c r="J4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
       <c r="N4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
       <c r="Q4" s="3" t="s">
         <v>51</v>
       </c>
@@ -6282,11 +6293,11 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="E5" s="6">
-        <f>'CF Adjustment'!G3</f>
-        <v>0.47356251901429836</v>
+        <f>'CF Adjustment'!H3</f>
+        <v>0.48469966657792307</v>
       </c>
       <c r="F5" s="5">
-        <v>6800</v>
+        <v>7480.0000000000009</v>
       </c>
       <c r="G5" s="5">
         <v>600</v>
@@ -6308,7 +6319,7 @@
       </c>
       <c r="N5" s="6">
         <f>E5</f>
-        <v>0.47356251901429836</v>
+        <v>0.48469966657792307</v>
       </c>
       <c r="O5" s="5">
         <v>6800</v>
@@ -6316,14 +6327,17 @@
       <c r="P5" s="5">
         <v>600</v>
       </c>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="7">
+        <f>$N5*8670*$G5*H5*F5/(2000*10^3)</f>
+        <v>215.00547445578673</v>
+      </c>
       <c r="R5" s="7">
         <f>$N5*8670*$G5*I5*F5/(2000*10^3)</f>
-        <v>6.1980961153635485</v>
-      </c>
-      <c r="S5" s="40">
-        <f>$D5*8670*$G5*J5*F5/(2000*10^3)</f>
-        <v>552517.94520000007</v>
+        <v>6.9782478551439553</v>
+      </c>
+      <c r="S5" s="7">
+        <f>$N5*8670*$G5*J5*F5/(2000*10^3)</f>
+        <v>1103317.5662862742</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6337,8 +6351,8 @@
         <v>0.314</v>
       </c>
       <c r="E6" s="6">
-        <f>'CF Adjustment'!G4</f>
-        <v>0.56870610177114023</v>
+        <f>'CF Adjustment'!H4</f>
+        <v>0.59940362701921202</v>
       </c>
       <c r="F6" s="5">
         <v>6400</v>
@@ -6363,7 +6377,7 @@
       </c>
       <c r="N6" s="6">
         <f>E6</f>
-        <v>0.56870610177114023</v>
+        <v>0.59940362701921202</v>
       </c>
       <c r="O6" s="5">
         <v>6400</v>
@@ -6373,11 +6387,11 @@
       </c>
       <c r="Q6" s="7">
         <f>$N6*8670*$G6*H6*F6/(2000*10^3)</f>
-        <v>165.48157373410396</v>
+        <v>174.41391114348446</v>
       </c>
       <c r="R6" s="7">
         <f>$N6*8670*$G6*I6*F6/(2000*10^3)</f>
-        <v>5.3708931825981105</v>
+        <v>5.6608023792183539</v>
       </c>
       <c r="S6" s="40">
         <f>$D6*8670*$G6*J6*F6/(2000*10^3)</f>
@@ -6395,8 +6409,8 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="E7" s="6">
-        <f>'CF Adjustment'!G5</f>
-        <v>0.62332721119862367</v>
+        <f>'CF Adjustment'!H5</f>
+        <v>0.66566575872790124</v>
       </c>
       <c r="F7" s="5">
         <v>6200</v>
@@ -6421,7 +6435,7 @@
       </c>
       <c r="N7" s="6">
         <f>E7</f>
-        <v>0.62332721119862367</v>
+        <v>0.66566575872790124</v>
       </c>
       <c r="O7" s="5">
         <v>6200</v>
@@ -6431,11 +6445,11 @@
       </c>
       <c r="Q7" s="7">
         <f>$N7*8670*$G7*H7*F7/(2000*10^3)</f>
-        <v>154.69872981502886</v>
+        <v>165.20640444774338</v>
       </c>
       <c r="R7" s="7">
         <f>$N7*8670*$G7*I7*F7/(2000*10^3)</f>
-        <v>5.0209236869790068</v>
+        <v>5.361962249619741</v>
       </c>
       <c r="S7" s="40">
         <f>$D7*8670*$G7*J7*F7/(2000*10^3)</f>
@@ -6453,8 +6467,8 @@
         <v>0.105</v>
       </c>
       <c r="E8" s="6">
-        <f>'CF Adjustment'!G6</f>
-        <v>0.20687557042896301</v>
+        <f>'CF Adjustment'!H6</f>
+        <v>0.39456636113540999</v>
       </c>
       <c r="F8" s="8">
         <v>8840</v>
@@ -6479,7 +6493,7 @@
       </c>
       <c r="N8" s="6">
         <f>E8</f>
-        <v>0.20687557042896301</v>
+        <v>0.39456636113540999</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>16</v>
@@ -6489,11 +6503,11 @@
       </c>
       <c r="Q8" s="7">
         <f>$N8*8670*$G8*H8*F8/(2000*10^3)</f>
-        <v>1120.1926977791322</v>
+        <v>2136.503385183129</v>
       </c>
       <c r="R8" s="7">
         <f>$N8*8670*$G8*I8*F8/(2000*10^3)</f>
-        <v>5.5262839757103857</v>
+        <v>10.540083366903435</v>
       </c>
       <c r="S8" s="40">
         <f>$D8*8670*$G8*J8*F8/(2000*10^3)</f>
@@ -6511,8 +6525,8 @@
         <v>0.105</v>
       </c>
       <c r="E9" s="6">
-        <f>'CF Adjustment'!G7</f>
-        <v>0.20687557042896301</v>
+        <f>'CF Adjustment'!H7</f>
+        <v>0.39456636113540999</v>
       </c>
       <c r="F9" s="8">
         <v>8840</v>
@@ -6537,7 +6551,7 @@
       </c>
       <c r="N9" s="6">
         <f>E9</f>
-        <v>0.20687557042896301</v>
+        <v>0.39456636113540999</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>16</v>
@@ -6547,11 +6561,11 @@
       </c>
       <c r="Q9" s="7">
         <f>$N9*8670*$G9*H9*F9/(2000*10^3)</f>
-        <v>170.26929006242813</v>
+        <v>324.74851454783567</v>
       </c>
       <c r="R9" s="7">
         <f>$N9*8670*$G9*I9*F9/(2000*10^3)</f>
-        <v>5.5262839757103857</v>
+        <v>10.540083366903435</v>
       </c>
       <c r="S9" s="40">
         <f>$D9*8670*$G9*J9*F9/(2000*10^3)</f>
@@ -6567,48 +6581,48 @@
       </c>
     </row>
     <row r="13" spans="2:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="57"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="19"/>
       <c r="L13" s="16"/>
     </row>
     <row r="14" spans="2:19" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="52" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="70" t="s">
+      <c r="F14" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="71"/>
-      <c r="H14" s="70" t="s">
+      <c r="G14" s="70"/>
+      <c r="H14" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="70"/>
     </row>
     <row r="15" spans="2:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="54"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="3" t="s">
         <v>18</v>
       </c>
@@ -6633,7 +6647,7 @@
       </c>
       <c r="D16" s="6">
         <f>E5</f>
-        <v>0.47356251901429836</v>
+        <v>0.48469966657792307</v>
       </c>
       <c r="E16" s="5">
         <v>600</v>
@@ -6643,14 +6657,14 @@
       </c>
       <c r="G16" s="7">
         <f>$D16*8760*$E16*F16/10^6</f>
-        <v>497.80891998783039</v>
+        <v>509.51628950671272</v>
       </c>
       <c r="H16" s="5">
         <v>250</v>
       </c>
       <c r="I16" s="7">
         <f>$D16*8760*$E16*H16/10^6</f>
-        <v>622.26114998478806</v>
+        <v>636.89536188339093</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6662,7 +6676,7 @@
       </c>
       <c r="D17" s="6">
         <f>E6</f>
-        <v>0.56870610177114023</v>
+        <v>0.59940362701921202</v>
       </c>
       <c r="E17" s="5">
         <v>460</v>
@@ -6672,14 +6686,14 @@
       </c>
       <c r="G17" s="7">
         <f>$D17*8760*$E17*F17/10^6</f>
-        <v>458.33162153939736</v>
+        <v>483.07137108732331</v>
       </c>
       <c r="H17" s="5">
         <v>250</v>
       </c>
       <c r="I17" s="7">
         <f>$D17*8760*$E17*H17/10^6</f>
-        <v>572.91452692424662</v>
+        <v>603.83921385915414</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6691,7 +6705,7 @@
       </c>
       <c r="D18" s="6">
         <f>E7</f>
-        <v>0.62332721119862367</v>
+        <v>0.66566575872790124</v>
       </c>
       <c r="E18" s="5">
         <v>405</v>
@@ -6701,14 +6715,14 @@
       </c>
       <c r="G18" s="7">
         <f>$D18*8760*$E18*F18/10^6</f>
-        <v>442.28805597809543</v>
+        <v>472.32979576296958</v>
       </c>
       <c r="H18" s="5">
         <v>250</v>
       </c>
       <c r="I18" s="7">
         <f>$D18*8760*$E18*H18/10^6</f>
-        <v>552.86006997261927</v>
+        <v>590.41224470371196</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6720,7 +6734,7 @@
       </c>
       <c r="D19" s="6">
         <f>E8</f>
-        <v>0.20687557042896301</v>
+        <v>0.39456636113540999</v>
       </c>
       <c r="E19" s="36">
         <v>942</v>
@@ -6730,27 +6744,27 @@
       </c>
       <c r="G19" s="37">
         <f>$D19*8760*$E19*F19/10^6</f>
-        <v>341.4241314268337</v>
+        <v>651.18600935610255</v>
       </c>
       <c r="H19" s="36">
         <v>250</v>
       </c>
       <c r="I19" s="37">
         <f>$D19*8760*$E19*H19/10^6</f>
-        <v>426.78016428354209</v>
+        <v>813.98251169512821</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="64"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="63"/>
       <c r="J20" s="34"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6759,25 +6773,25 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="69"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
       <c r="I23" s="39"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="59" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="38" t="s">
@@ -6786,15 +6800,15 @@
       <c r="F24" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="65" t="s">
+      <c r="G24" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="66"/>
+      <c r="H24" s="65"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="59"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
       <c r="E25" s="11" t="s">
         <v>31</v>
       </c>
@@ -6939,893 +6953,1035 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC5736E-F416-4A91-98C0-BF05C38E1A71}">
-  <dimension ref="A1:N13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B724EB-6910-45D9-ADF5-6C5EE28B5832}">
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B2" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F2" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G2" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="I2" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="J2" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="K2" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="L2" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M2" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N2" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O2" s="43" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43" t="s">
+      <c r="P2" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F3" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G3" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="I3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="J3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="K3" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="L3" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="M3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="N3" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="O3" s="43" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="P3" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="S3" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="W3" s="82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="75">
-        <v>0.38667477943413398</v>
-      </c>
-      <c r="E3" s="45">
-        <f>'CF Adjustment'!G3</f>
-        <v>0.47356251901429836</v>
-      </c>
-      <c r="F3" s="46">
-        <v>6800</v>
-      </c>
-      <c r="G3">
-        <v>600</v>
-      </c>
-      <c r="H3" s="44"/>
-      <c r="I3">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="J3">
-        <f>I3*F3/(10^3)</f>
-        <v>0.15503999999999998</v>
-      </c>
-      <c r="K3">
-        <f>J3*G3*8670*E3/2000</f>
-        <v>190.96836679768765</v>
-      </c>
-      <c r="L3">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>12</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="75">
-        <v>0.470946151505932</v>
-      </c>
-      <c r="E4" s="45">
-        <f>'CF Adjustment'!G4</f>
-        <v>0.56870610177114023</v>
+      <c r="D4" s="74">
+        <v>0.39965009698398801</v>
+      </c>
+      <c r="E4" s="76">
+        <f>'CF Adjustment'!I3</f>
+        <v>0.48469966657792307</v>
       </c>
       <c r="F4" s="46">
-        <v>6400</v>
-      </c>
-      <c r="G4">
-        <v>460</v>
-      </c>
-      <c r="H4" s="44"/>
-      <c r="I4">
+        <v>6800</v>
+      </c>
+      <c r="G4" s="46">
+        <f>F4*1.1</f>
+        <v>7480.0000000000009</v>
+      </c>
+      <c r="H4" s="44">
+        <v>600</v>
+      </c>
+      <c r="I4" s="44"/>
+      <c r="J4">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J11" si="0">I4*F4/(10^3)</f>
-        <v>0.14592000000000002</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K11" si="1">J4*G4*8670*E4/2000</f>
-        <v>165.48157373410396</v>
-      </c>
-      <c r="L4">
+      <c r="K4" s="80">
+        <f>J4*G4/(10^3)</f>
+        <v>0.17054400000000003</v>
+      </c>
+      <c r="L4" s="80">
+        <f>K4*H4*8670*E4/2000</f>
+        <v>215.00547445578673</v>
+      </c>
+      <c r="M4">
         <v>7.3999999999999999E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="79">
+        <f>M4*G4/(10^3)</f>
+        <v>5.5352000000000005E-3</v>
+      </c>
+      <c r="O4" s="80">
+        <f>N4*H4*8670*E4/2000</f>
+        <v>6.9782478551439544</v>
+      </c>
+      <c r="P4" s="19">
+        <v>117</v>
+      </c>
+      <c r="Q4">
+        <f>P4*G4/(10^3)</f>
+        <v>875.16000000000008</v>
+      </c>
+      <c r="R4" s="81">
+        <f>Q4*H4*8670*E4/2000</f>
+        <v>1103317.5662862738</v>
+      </c>
+      <c r="S4" s="44"/>
+      <c r="T4" s="19">
+        <v>200</v>
+      </c>
+      <c r="U4" s="81">
+        <f>$E4*8760*$T4*H4/10^6</f>
+        <v>509.51628950671278</v>
+      </c>
+      <c r="V4" s="19">
+        <v>250</v>
+      </c>
+      <c r="W4" s="81">
+        <f>$E4*8760*$V4*H4/10^6</f>
+        <v>636.89536188339105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="75">
-        <v>0.52327350167325803</v>
-      </c>
-      <c r="E5" s="45">
-        <f>'CF Adjustment'!G5</f>
-        <v>0.62332721119862367</v>
+      <c r="D5" s="74">
+        <v>0.50860178247690002</v>
+      </c>
+      <c r="E5" s="76">
+        <f>'CF Adjustment'!I4</f>
+        <v>0.59940362701921202</v>
       </c>
       <c r="F5" s="46">
+        <v>6400</v>
+      </c>
+      <c r="G5" s="46">
+        <f t="shared" ref="G5:G8" si="0">F5*1.1</f>
+        <v>7040.0000000000009</v>
+      </c>
+      <c r="H5" s="44">
+        <v>460</v>
+      </c>
+      <c r="I5" s="44"/>
+      <c r="J5">
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="K5" s="80">
+        <f t="shared" ref="K5:K8" si="1">J5*G5/(10^3)</f>
+        <v>0.16051200000000002</v>
+      </c>
+      <c r="L5" s="80">
+        <f t="shared" ref="L5:L12" si="2">K5*H5*8670*E5/2000</f>
+        <v>191.8553022578329</v>
+      </c>
+      <c r="M5">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="N5" s="79">
+        <f t="shared" ref="N5:N8" si="3">M5*G5/(10^3)</f>
+        <v>5.2096000000000009E-3</v>
+      </c>
+      <c r="O5" s="80">
+        <f t="shared" ref="O5:O8" si="4">N5*H5*8670*E5/2000</f>
+        <v>6.2268826171401903</v>
+      </c>
+      <c r="P5" s="19">
+        <v>117</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q8" si="5">P5*G5/(10^3)</f>
+        <v>823.68000000000006</v>
+      </c>
+      <c r="R5" s="81">
+        <f t="shared" ref="R5:R8" si="6">Q5*H5*8670*E5/2000</f>
+        <v>984520.63000730053</v>
+      </c>
+      <c r="S5" s="44"/>
+      <c r="T5" s="19">
+        <v>200</v>
+      </c>
+      <c r="U5" s="81">
+        <f t="shared" ref="U5:U8" si="7">$E5*8760*$T5*H5/10^6</f>
+        <v>483.07137108732331</v>
+      </c>
+      <c r="V5" s="19">
+        <v>250</v>
+      </c>
+      <c r="W5" s="81">
+        <f t="shared" ref="W5:W8" si="8">$E5*8760*$V5*H5/10^6</f>
+        <v>603.83921385915426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="74">
+        <v>0.57685822589000002</v>
+      </c>
+      <c r="E6" s="76">
+        <f>'CF Adjustment'!I5</f>
+        <v>0.66566575872790124</v>
+      </c>
+      <c r="F6" s="46">
         <v>6200</v>
       </c>
-      <c r="G5">
+      <c r="G6" s="46">
+        <f t="shared" si="0"/>
+        <v>6820.0000000000009</v>
+      </c>
+      <c r="H6" s="44">
         <v>405</v>
       </c>
-      <c r="H5" s="44"/>
-      <c r="I5">
+      <c r="I6" s="44"/>
+      <c r="J6">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0.14136000000000001</v>
-      </c>
-      <c r="K5">
+      <c r="K6" s="80">
         <f t="shared" si="1"/>
-        <v>154.69872981502888</v>
-      </c>
-      <c r="L5">
+        <v>0.15549600000000005</v>
+      </c>
+      <c r="L6" s="80">
+        <f t="shared" si="2"/>
+        <v>181.72704489251777</v>
+      </c>
+      <c r="M6">
         <v>7.3999999999999999E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="N6" s="79">
+        <f t="shared" si="3"/>
+        <v>5.0468000000000006E-3</v>
+      </c>
+      <c r="O6" s="80">
+        <f t="shared" si="4"/>
+        <v>5.8981584745817166</v>
+      </c>
+      <c r="P6" s="19">
+        <v>117</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="5"/>
+        <v>797.94000000000017</v>
+      </c>
+      <c r="R6" s="81">
+        <f t="shared" si="6"/>
+        <v>932546.67773792008</v>
+      </c>
+      <c r="S6" s="44"/>
+      <c r="T6" s="19">
+        <v>200</v>
+      </c>
+      <c r="U6" s="81">
+        <f t="shared" si="7"/>
+        <v>472.32979576296964</v>
+      </c>
+      <c r="V6" s="19">
+        <v>250</v>
+      </c>
+      <c r="W6" s="81">
+        <f t="shared" si="8"/>
+        <v>590.41224470371196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="75">
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="E6" s="45">
-        <f>'CF Adjustment'!G6</f>
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="F6" s="47">
-        <v>7760</v>
-      </c>
-      <c r="G6">
-        <v>942</v>
-      </c>
-      <c r="H6" s="44"/>
-      <c r="I6">
-        <v>0.15</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.1639999999999999</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>983.3365763310029</v>
-      </c>
-      <c r="L6">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>66</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="75">
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="E7" s="45">
-        <f>'CF Adjustment'!G7</f>
-        <v>0.20687557042896301</v>
+      <c r="D7" s="74">
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="E7" s="76">
+        <f>'CF Adjustment'!I6</f>
+        <v>0.39456636113540999</v>
       </c>
       <c r="F7" s="47">
         <v>7760</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="46">
+        <f t="shared" si="0"/>
+        <v>8536</v>
+      </c>
+      <c r="H7" s="44">
         <v>942</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7">
+      <c r="I7" s="44"/>
+      <c r="J7">
+        <v>0.15</v>
+      </c>
+      <c r="K7" s="80">
+        <f t="shared" si="1"/>
+        <v>1.2803999999999998</v>
+      </c>
+      <c r="L7" s="80">
+        <f t="shared" si="2"/>
+        <v>2063.030870579546</v>
+      </c>
+      <c r="M7">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="N7" s="79">
+        <f t="shared" si="3"/>
+        <v>6.3166399999999992E-3</v>
+      </c>
+      <c r="O7" s="80">
+        <f t="shared" si="4"/>
+        <v>10.177618961525761</v>
+      </c>
+      <c r="P7" s="19">
+        <v>117</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>998.71199999999999</v>
+      </c>
+      <c r="R7" s="81">
+        <f t="shared" si="6"/>
+        <v>1609164.0790520462</v>
+      </c>
+      <c r="S7" s="44"/>
+      <c r="T7" s="19">
+        <v>200</v>
+      </c>
+      <c r="U7" s="81">
+        <f t="shared" si="7"/>
+        <v>651.18600935610243</v>
+      </c>
+      <c r="V7" s="19">
+        <v>250</v>
+      </c>
+      <c r="W7" s="81">
+        <f t="shared" si="8"/>
+        <v>813.9825116951281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="74">
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="E8" s="76">
+        <f>'CF Adjustment'!I7</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="F8" s="47">
+        <v>7760</v>
+      </c>
+      <c r="G8" s="46">
+        <f t="shared" si="0"/>
+        <v>8536</v>
+      </c>
+      <c r="H8" s="44">
+        <v>942</v>
+      </c>
+      <c r="I8" s="44"/>
+      <c r="J8">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>0.176928</v>
-      </c>
-      <c r="K7">
+      <c r="K8" s="80">
         <f t="shared" si="1"/>
-        <v>149.46715960231245</v>
-      </c>
-      <c r="L7">
+        <v>0.19462080000000001</v>
+      </c>
+      <c r="L8" s="80">
+        <f t="shared" si="2"/>
+        <v>313.580692328091</v>
+      </c>
+      <c r="M8">
         <v>7.3999999999999999E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="N8" s="79">
+        <f t="shared" si="3"/>
+        <v>6.3166399999999992E-3</v>
+      </c>
+      <c r="O8" s="80">
+        <f t="shared" si="4"/>
+        <v>10.177618961525761</v>
+      </c>
+      <c r="P8" s="19">
+        <v>117</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>998.71199999999999</v>
+      </c>
+      <c r="R8" s="81">
+        <f t="shared" si="6"/>
+        <v>1609164.0790520462</v>
+      </c>
+      <c r="S8" s="44"/>
+      <c r="T8" s="19">
+        <v>200</v>
+      </c>
+      <c r="U8" s="81">
+        <f t="shared" si="7"/>
+        <v>651.18600935610243</v>
+      </c>
+      <c r="V8" s="19">
+        <v>250</v>
+      </c>
+      <c r="W8" s="81">
+        <f t="shared" si="8"/>
+        <v>813.9825116951281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B9" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C9" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D9" s="74">
         <f>'CF Adjustment'!C12*0.203+'CF Adjustment'!C11*0.702</f>
         <v>0.32774999999999999</v>
       </c>
-      <c r="E8" s="45">
-        <f>D8</f>
+      <c r="E9" s="45">
+        <f>D9</f>
         <v>0.32774999999999999</v>
       </c>
-      <c r="G8">
+      <c r="H9">
         <v>250</v>
       </c>
-      <c r="H8" s="44">
+      <c r="I9" s="44">
         <v>8000</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
+      <c r="K9">
+        <f t="shared" ref="K5:K12" si="9">J9*F9/(10^3)</f>
         <v>0</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
+      <c r="L9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="Q9">
+        <v>55</v>
+      </c>
+      <c r="R9" s="80">
+        <f>E9*Q9*8760*H9/(10^6)</f>
+        <v>39.477487499999995</v>
+      </c>
+      <c r="S9" s="44">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B10" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D10" s="74">
         <f>0.53*'CF Adjustment'!C15+0.342*'CF Adjustment'!C16+0.49*'CF Adjustment'!C17+0.53*'CF Adjustment'!C18</f>
         <v>0.49533333333333335</v>
       </c>
-      <c r="E9" s="45">
-        <f t="shared" ref="E9:E11" si="2">D9</f>
+      <c r="E10" s="45">
+        <f t="shared" ref="E10:E12" si="10">D10</f>
         <v>0.49533333333333335</v>
       </c>
-      <c r="G9">
+      <c r="H10">
         <v>250</v>
       </c>
-      <c r="H9" s="44">
+      <c r="I10" s="44">
         <v>38000</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
+      <c r="K10">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
+      <c r="L10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="Q10">
+        <v>13</v>
+      </c>
+      <c r="R10" s="80">
+        <f t="shared" ref="R10:R12" si="11">E10*Q10*8760*H10/(10^6)</f>
+        <v>14.102140000000002</v>
+      </c>
+      <c r="S10" s="44">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B11" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C11" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D11" s="74">
         <f>0.498*'CF Adjustment'!C12+0.435*'CF Adjustment'!C16+0.456*'CF Adjustment'!C17</f>
         <v>0.48399999999999999</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E11" s="45">
+        <f t="shared" si="10"/>
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="H11">
+        <v>200</v>
+      </c>
+      <c r="I11" s="44">
+        <v>20000</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="2"/>
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="G10">
-        <v>200</v>
-      </c>
-      <c r="H10" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>13</v>
+      </c>
+      <c r="R11" s="80">
+        <f t="shared" si="11"/>
+        <v>11.023584</v>
+      </c>
+      <c r="S11" s="44">
         <v>20000</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B12" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C12" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="76">
+      <c r="D12" s="74">
         <f>0.454*'CF Adjustment'!C12+0.419*'CF Adjustment'!C16+0.428*'CF Adjustment'!C17</f>
         <v>0.44600000000000006</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E12" s="45">
+        <f t="shared" si="10"/>
+        <v>0.44600000000000006</v>
+      </c>
+      <c r="H12">
+        <v>150</v>
+      </c>
+      <c r="I12" s="44">
+        <v>20000</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="2"/>
-        <v>0.44600000000000006</v>
-      </c>
-      <c r="G11">
-        <v>150</v>
-      </c>
-      <c r="H11" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>13</v>
+      </c>
+      <c r="R12" s="80">
+        <f t="shared" si="11"/>
+        <v>7.6185720000000021</v>
+      </c>
+      <c r="S12" s="44">
         <v>20000</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="44"/>
-      <c r="H12" s="44"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H13" s="44"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="S13" s="44"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I14" s="44"/>
+      <c r="S14" s="44"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T15" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B724EB-6910-45D9-ADF5-6C5EE28B5832}">
-  <dimension ref="A1:N13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5564981C-E4C1-4223-BBB8-B7B238FE5FB5}">
+  <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+    <row r="2" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="29">
+        <f>LCA_Hourly!D4</f>
+        <v>0.39965009698398801</v>
+      </c>
+      <c r="D3" s="29">
+        <f>LCA_Hourly!D4</f>
+        <v>0.39965009698398801</v>
+      </c>
+      <c r="E3" s="28">
+        <v>600</v>
+      </c>
+      <c r="F3" s="27">
+        <v>85</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="76">
-        <v>0.27397659706639299</v>
-      </c>
-      <c r="E3" s="78">
-        <f>'CF Adjustment'!G3</f>
-        <v>0.47356251901429836</v>
-      </c>
-      <c r="F3" s="46">
-        <v>6800</v>
-      </c>
-      <c r="G3" s="44">
-        <v>600</v>
-      </c>
-      <c r="H3" s="44"/>
-      <c r="I3">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="J3">
-        <f>I3*F3/(10^3)</f>
-        <v>0.15503999999999998</v>
-      </c>
-      <c r="K3">
-        <f>J3*G3*8670*E3/2000</f>
-        <v>190.96836679768765</v>
-      </c>
-      <c r="L3">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="H3" s="33">
+        <f>C3*(1-(F3/E3))+(F3/E3)</f>
+        <v>0.48469966657792307</v>
+      </c>
+      <c r="I3" s="33">
+        <f>D3*(1-(F3/E3))+(F3/E3)</f>
+        <v>0.48469966657792307</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="29">
+        <f>LCA_Hourly!D5</f>
+        <v>0.50860178247690002</v>
+      </c>
+      <c r="D4" s="29">
+        <f>LCA_Hourly!D5</f>
+        <v>0.50860178247690002</v>
+      </c>
+      <c r="E4" s="28">
+        <v>460</v>
+      </c>
+      <c r="F4" s="27">
+        <v>85</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="76">
-        <v>0.32037677962448802</v>
-      </c>
-      <c r="E4" s="78">
-        <f>'CF Adjustment'!G4</f>
-        <v>0.56870610177114023</v>
-      </c>
-      <c r="F4" s="46">
-        <v>6400</v>
-      </c>
-      <c r="G4" s="44">
-        <v>460</v>
-      </c>
-      <c r="H4" s="44"/>
-      <c r="I4">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J11" si="0">I4*F4/(10^3)</f>
-        <v>0.14592000000000002</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K11" si="1">J4*G4*8670*E4/2000</f>
-        <v>165.48157373410396</v>
-      </c>
-      <c r="L4">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="H4" s="33">
+        <f>C4*(1-(F4/E4))+(F4/E4)</f>
+        <v>0.59940362701921202</v>
+      </c>
+      <c r="I4" s="33">
+        <f t="shared" ref="I4:I7" si="0">D4*(1-(F4/E4))+(F4/E4)</f>
+        <v>0.59940362701921202</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="C5" s="29">
+        <f>LCA_Hourly!D6</f>
+        <v>0.57685822589000002</v>
+      </c>
+      <c r="D5" s="29">
+        <f>LCA_Hourly!D6</f>
+        <v>0.57685822589000002</v>
+      </c>
+      <c r="E5" s="28">
+        <v>405</v>
+      </c>
+      <c r="F5" s="27">
+        <v>85</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="76">
-        <v>0.35030870066811198</v>
-      </c>
-      <c r="E5" s="78">
-        <f>'CF Adjustment'!G5</f>
-        <v>0.62332721119862367</v>
-      </c>
-      <c r="F5" s="46">
-        <v>6200</v>
-      </c>
-      <c r="G5" s="44">
-        <v>405</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="J5">
+      <c r="H5" s="33">
+        <f>C5*(1-(F5/E5))+(F5/E5)</f>
+        <v>0.66566575872790124</v>
+      </c>
+      <c r="I5" s="33">
         <f t="shared" si="0"/>
-        <v>0.14136000000000001</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>154.69872981502888</v>
-      </c>
-      <c r="L5">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="76">
-        <v>0.185207723221643</v>
-      </c>
-      <c r="E6" s="78">
-        <f>'CF Adjustment'!G6</f>
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="F6" s="47">
-        <v>7760</v>
-      </c>
-      <c r="G6" s="44">
+        <v>0.66566575872790124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="29">
+        <f>LCA_Hourly!D7</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="D6" s="29">
+        <f>LCA_Hourly!D7</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="E6" s="28">
         <v>942</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6">
-        <v>0.15</v>
-      </c>
-      <c r="J6">
+      <c r="F6" s="27">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="33">
+        <f>C6*(1-(F6/E6))+(F6/E6)</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="I6" s="33">
         <f t="shared" si="0"/>
-        <v>1.1639999999999999</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>983.3365763310029</v>
-      </c>
-      <c r="L6">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="76">
-        <v>0.185207723221643</v>
-      </c>
-      <c r="E7" s="78">
-        <f>'CF Adjustment'!G7</f>
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="F7" s="47">
-        <v>7760</v>
-      </c>
-      <c r="G7" s="44">
+        <v>0.39456636113540999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="29">
+        <f>LCA_Hourly!D8</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="D7" s="29">
+        <f>LCA_Hourly!D8</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="E7" s="28">
         <v>942</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="J7">
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="33">
+        <f>C7*(1-(F7/E7))+(F7/E7)</f>
+        <v>0.39456636113540999</v>
+      </c>
+      <c r="I7" s="33">
         <f t="shared" si="0"/>
-        <v>0.176928</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>149.46715960231245</v>
-      </c>
-      <c r="L7">
-        <v>7.3999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="76">
-        <f>'CF Adjustment'!C12*0.203+'CF Adjustment'!C11*0.702</f>
-        <v>0.32774999999999999</v>
-      </c>
-      <c r="E8" s="45">
-        <f>D8</f>
-        <v>0.32774999999999999</v>
-      </c>
-      <c r="G8">
-        <v>250</v>
-      </c>
-      <c r="H8" s="44">
-        <v>8000</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="76">
-        <f>0.53*'CF Adjustment'!C15+0.342*'CF Adjustment'!C16+0.49*'CF Adjustment'!C17+0.53*'CF Adjustment'!C18</f>
-        <v>0.49533333333333335</v>
-      </c>
-      <c r="E9" s="45">
-        <f t="shared" ref="E9:E11" si="2">D9</f>
-        <v>0.49533333333333335</v>
-      </c>
-      <c r="G9">
-        <v>250</v>
-      </c>
-      <c r="H9" s="44">
-        <v>38000</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="76">
-        <f>0.498*'CF Adjustment'!C12+0.435*'CF Adjustment'!C16+0.456*'CF Adjustment'!C17</f>
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="E10" s="45">
-        <f t="shared" si="2"/>
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="G10">
-        <v>200</v>
-      </c>
-      <c r="H10" s="44">
-        <v>20000</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="76">
-        <f>0.454*'CF Adjustment'!C12+0.419*'CF Adjustment'!C16+0.428*'CF Adjustment'!C17</f>
-        <v>0.44600000000000006</v>
-      </c>
-      <c r="E11" s="45">
-        <f t="shared" si="2"/>
-        <v>0.44600000000000006</v>
-      </c>
-      <c r="G11">
-        <v>150</v>
-      </c>
-      <c r="H11" s="44">
-        <v>20000</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.39456636113540999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="72"/>
+      <c r="D10" s="77"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="44"/>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="15">
+        <v>0.75</v>
+      </c>
       <c r="D12" s="44"/>
-      <c r="H12" s="44"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H13" s="44"/>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="72"/>
+      <c r="D14" s="77"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="13">
+        <f>C12*(22/24)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="D15" s="44"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="13">
+        <f>C11-C17</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="D16" s="44"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="13">
+        <f>C11*(8/24)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D17" s="44"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="15">
+        <f>C12-C15</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D18" s="44"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7869,7 +8025,7 @@
       <c r="B2">
         <v>2011</v>
       </c>
-      <c r="C2" s="74">
+      <c r="C2" s="73">
         <f>DATE(B2,A2,1)</f>
         <v>40544</v>
       </c>
@@ -7893,7 +8049,7 @@
       <c r="B3">
         <v>2011</v>
       </c>
-      <c r="C3" s="74">
+      <c r="C3" s="73">
         <f t="shared" ref="C3:C66" si="0">DATE(B3,A3,1)</f>
         <v>40575</v>
       </c>
@@ -7917,7 +8073,7 @@
       <c r="B4">
         <v>2011</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C4" s="73">
         <f t="shared" si="0"/>
         <v>40603</v>
       </c>
@@ -7941,7 +8097,7 @@
       <c r="B5">
         <v>2011</v>
       </c>
-      <c r="C5" s="74">
+      <c r="C5" s="73">
         <f t="shared" si="0"/>
         <v>40634</v>
       </c>
@@ -7965,7 +8121,7 @@
       <c r="B6">
         <v>2011</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="73">
         <f t="shared" si="0"/>
         <v>40664</v>
       </c>
@@ -7989,7 +8145,7 @@
       <c r="B7">
         <v>2011</v>
       </c>
-      <c r="C7" s="74">
+      <c r="C7" s="73">
         <f t="shared" si="0"/>
         <v>40695</v>
       </c>
@@ -8013,7 +8169,7 @@
       <c r="B8">
         <v>2011</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C8" s="73">
         <f t="shared" si="0"/>
         <v>40725</v>
       </c>
@@ -8037,7 +8193,7 @@
       <c r="B9">
         <v>2011</v>
       </c>
-      <c r="C9" s="74">
+      <c r="C9" s="73">
         <f t="shared" si="0"/>
         <v>40756</v>
       </c>
@@ -8061,7 +8217,7 @@
       <c r="B10">
         <v>2011</v>
       </c>
-      <c r="C10" s="74">
+      <c r="C10" s="73">
         <f t="shared" si="0"/>
         <v>40787</v>
       </c>
@@ -8085,7 +8241,7 @@
       <c r="B11">
         <v>2011</v>
       </c>
-      <c r="C11" s="74">
+      <c r="C11" s="73">
         <f t="shared" si="0"/>
         <v>40817</v>
       </c>
@@ -8109,7 +8265,7 @@
       <c r="B12">
         <v>2011</v>
       </c>
-      <c r="C12" s="74">
+      <c r="C12" s="73">
         <f t="shared" si="0"/>
         <v>40848</v>
       </c>
@@ -8133,7 +8289,7 @@
       <c r="B13">
         <v>2011</v>
       </c>
-      <c r="C13" s="74">
+      <c r="C13" s="73">
         <f t="shared" si="0"/>
         <v>40878</v>
       </c>
@@ -8157,7 +8313,7 @@
       <c r="B14">
         <v>2012</v>
       </c>
-      <c r="C14" s="74">
+      <c r="C14" s="73">
         <f t="shared" si="0"/>
         <v>40909</v>
       </c>
@@ -8181,7 +8337,7 @@
       <c r="B15">
         <v>2012</v>
       </c>
-      <c r="C15" s="74">
+      <c r="C15" s="73">
         <f t="shared" si="0"/>
         <v>40940</v>
       </c>
@@ -8205,7 +8361,7 @@
       <c r="B16">
         <v>2012</v>
       </c>
-      <c r="C16" s="74">
+      <c r="C16" s="73">
         <f t="shared" si="0"/>
         <v>40969</v>
       </c>
@@ -8229,7 +8385,7 @@
       <c r="B17">
         <v>2012</v>
       </c>
-      <c r="C17" s="74">
+      <c r="C17" s="73">
         <f t="shared" si="0"/>
         <v>41000</v>
       </c>
@@ -8253,7 +8409,7 @@
       <c r="B18">
         <v>2012</v>
       </c>
-      <c r="C18" s="74">
+      <c r="C18" s="73">
         <f t="shared" si="0"/>
         <v>41030</v>
       </c>
@@ -8277,7 +8433,7 @@
       <c r="B19">
         <v>2012</v>
       </c>
-      <c r="C19" s="74">
+      <c r="C19" s="73">
         <f t="shared" si="0"/>
         <v>41061</v>
       </c>
@@ -8301,7 +8457,7 @@
       <c r="B20">
         <v>2012</v>
       </c>
-      <c r="C20" s="74">
+      <c r="C20" s="73">
         <f t="shared" si="0"/>
         <v>41091</v>
       </c>
@@ -8325,7 +8481,7 @@
       <c r="B21">
         <v>2012</v>
       </c>
-      <c r="C21" s="74">
+      <c r="C21" s="73">
         <f t="shared" si="0"/>
         <v>41122</v>
       </c>
@@ -8349,7 +8505,7 @@
       <c r="B22">
         <v>2012</v>
       </c>
-      <c r="C22" s="74">
+      <c r="C22" s="73">
         <f t="shared" si="0"/>
         <v>41153</v>
       </c>
@@ -8373,7 +8529,7 @@
       <c r="B23">
         <v>2012</v>
       </c>
-      <c r="C23" s="74">
+      <c r="C23" s="73">
         <f t="shared" si="0"/>
         <v>41183</v>
       </c>
@@ -8397,7 +8553,7 @@
       <c r="B24">
         <v>2012</v>
       </c>
-      <c r="C24" s="74">
+      <c r="C24" s="73">
         <f t="shared" si="0"/>
         <v>41214</v>
       </c>
@@ -8421,7 +8577,7 @@
       <c r="B25">
         <v>2012</v>
       </c>
-      <c r="C25" s="74">
+      <c r="C25" s="73">
         <f t="shared" si="0"/>
         <v>41244</v>
       </c>
@@ -8445,7 +8601,7 @@
       <c r="B26">
         <v>2013</v>
       </c>
-      <c r="C26" s="74">
+      <c r="C26" s="73">
         <f t="shared" si="0"/>
         <v>41275</v>
       </c>
@@ -8469,7 +8625,7 @@
       <c r="B27">
         <v>2013</v>
       </c>
-      <c r="C27" s="74">
+      <c r="C27" s="73">
         <f t="shared" si="0"/>
         <v>41306</v>
       </c>
@@ -8493,7 +8649,7 @@
       <c r="B28">
         <v>2013</v>
       </c>
-      <c r="C28" s="74">
+      <c r="C28" s="73">
         <f t="shared" si="0"/>
         <v>41334</v>
       </c>
@@ -8517,7 +8673,7 @@
       <c r="B29">
         <v>2013</v>
       </c>
-      <c r="C29" s="74">
+      <c r="C29" s="73">
         <f t="shared" si="0"/>
         <v>41365</v>
       </c>
@@ -8541,7 +8697,7 @@
       <c r="B30">
         <v>2013</v>
       </c>
-      <c r="C30" s="74">
+      <c r="C30" s="73">
         <f t="shared" si="0"/>
         <v>41395</v>
       </c>
@@ -8565,7 +8721,7 @@
       <c r="B31">
         <v>2013</v>
       </c>
-      <c r="C31" s="74">
+      <c r="C31" s="73">
         <f t="shared" si="0"/>
         <v>41426</v>
       </c>
@@ -8589,7 +8745,7 @@
       <c r="B32">
         <v>2013</v>
       </c>
-      <c r="C32" s="74">
+      <c r="C32" s="73">
         <f t="shared" si="0"/>
         <v>41456</v>
       </c>
@@ -8613,7 +8769,7 @@
       <c r="B33">
         <v>2013</v>
       </c>
-      <c r="C33" s="74">
+      <c r="C33" s="73">
         <f t="shared" si="0"/>
         <v>41487</v>
       </c>
@@ -8637,7 +8793,7 @@
       <c r="B34">
         <v>2013</v>
       </c>
-      <c r="C34" s="74">
+      <c r="C34" s="73">
         <f t="shared" si="0"/>
         <v>41518</v>
       </c>
@@ -8661,7 +8817,7 @@
       <c r="B35">
         <v>2013</v>
       </c>
-      <c r="C35" s="74">
+      <c r="C35" s="73">
         <f t="shared" si="0"/>
         <v>41548</v>
       </c>
@@ -8685,7 +8841,7 @@
       <c r="B36">
         <v>2013</v>
       </c>
-      <c r="C36" s="74">
+      <c r="C36" s="73">
         <f t="shared" si="0"/>
         <v>41579</v>
       </c>
@@ -8709,7 +8865,7 @@
       <c r="B37">
         <v>2013</v>
       </c>
-      <c r="C37" s="74">
+      <c r="C37" s="73">
         <f t="shared" si="0"/>
         <v>41609</v>
       </c>
@@ -8733,7 +8889,7 @@
       <c r="B38">
         <v>2014</v>
       </c>
-      <c r="C38" s="74">
+      <c r="C38" s="73">
         <f t="shared" si="0"/>
         <v>41640</v>
       </c>
@@ -8757,7 +8913,7 @@
       <c r="B39">
         <v>2014</v>
       </c>
-      <c r="C39" s="74">
+      <c r="C39" s="73">
         <f t="shared" si="0"/>
         <v>41671</v>
       </c>
@@ -8781,7 +8937,7 @@
       <c r="B40">
         <v>2014</v>
       </c>
-      <c r="C40" s="74">
+      <c r="C40" s="73">
         <f t="shared" si="0"/>
         <v>41699</v>
       </c>
@@ -8805,7 +8961,7 @@
       <c r="B41">
         <v>2014</v>
       </c>
-      <c r="C41" s="74">
+      <c r="C41" s="73">
         <f t="shared" si="0"/>
         <v>41730</v>
       </c>
@@ -8829,7 +8985,7 @@
       <c r="B42">
         <v>2014</v>
       </c>
-      <c r="C42" s="74">
+      <c r="C42" s="73">
         <f t="shared" si="0"/>
         <v>41760</v>
       </c>
@@ -8853,7 +9009,7 @@
       <c r="B43">
         <v>2014</v>
       </c>
-      <c r="C43" s="74">
+      <c r="C43" s="73">
         <f t="shared" si="0"/>
         <v>41791</v>
       </c>
@@ -8877,7 +9033,7 @@
       <c r="B44">
         <v>2014</v>
       </c>
-      <c r="C44" s="74">
+      <c r="C44" s="73">
         <f t="shared" si="0"/>
         <v>41821</v>
       </c>
@@ -8901,7 +9057,7 @@
       <c r="B45">
         <v>2014</v>
       </c>
-      <c r="C45" s="74">
+      <c r="C45" s="73">
         <f t="shared" si="0"/>
         <v>41852</v>
       </c>
@@ -8925,7 +9081,7 @@
       <c r="B46">
         <v>2014</v>
       </c>
-      <c r="C46" s="74">
+      <c r="C46" s="73">
         <f t="shared" si="0"/>
         <v>41883</v>
       </c>
@@ -8949,7 +9105,7 @@
       <c r="B47">
         <v>2014</v>
       </c>
-      <c r="C47" s="74">
+      <c r="C47" s="73">
         <f t="shared" si="0"/>
         <v>41913</v>
       </c>
@@ -8973,7 +9129,7 @@
       <c r="B48">
         <v>2014</v>
       </c>
-      <c r="C48" s="74">
+      <c r="C48" s="73">
         <f t="shared" si="0"/>
         <v>41944</v>
       </c>
@@ -8997,7 +9153,7 @@
       <c r="B49">
         <v>2014</v>
       </c>
-      <c r="C49" s="74">
+      <c r="C49" s="73">
         <f t="shared" si="0"/>
         <v>41974</v>
       </c>
@@ -9021,7 +9177,7 @@
       <c r="B50">
         <v>2015</v>
       </c>
-      <c r="C50" s="74">
+      <c r="C50" s="73">
         <f t="shared" si="0"/>
         <v>42005</v>
       </c>
@@ -9045,7 +9201,7 @@
       <c r="B51">
         <v>2015</v>
       </c>
-      <c r="C51" s="74">
+      <c r="C51" s="73">
         <f t="shared" si="0"/>
         <v>42036</v>
       </c>
@@ -9069,7 +9225,7 @@
       <c r="B52">
         <v>2015</v>
       </c>
-      <c r="C52" s="74">
+      <c r="C52" s="73">
         <f t="shared" si="0"/>
         <v>42064</v>
       </c>
@@ -9093,7 +9249,7 @@
       <c r="B53">
         <v>2015</v>
       </c>
-      <c r="C53" s="74">
+      <c r="C53" s="73">
         <f t="shared" si="0"/>
         <v>42095</v>
       </c>
@@ -9117,7 +9273,7 @@
       <c r="B54">
         <v>2015</v>
       </c>
-      <c r="C54" s="74">
+      <c r="C54" s="73">
         <f t="shared" si="0"/>
         <v>42125</v>
       </c>
@@ -9141,7 +9297,7 @@
       <c r="B55">
         <v>2015</v>
       </c>
-      <c r="C55" s="74">
+      <c r="C55" s="73">
         <f t="shared" si="0"/>
         <v>42156</v>
       </c>
@@ -9165,7 +9321,7 @@
       <c r="B56">
         <v>2015</v>
       </c>
-      <c r="C56" s="74">
+      <c r="C56" s="73">
         <f t="shared" si="0"/>
         <v>42186</v>
       </c>
@@ -9189,7 +9345,7 @@
       <c r="B57">
         <v>2015</v>
       </c>
-      <c r="C57" s="74">
+      <c r="C57" s="73">
         <f t="shared" si="0"/>
         <v>42217</v>
       </c>
@@ -9213,7 +9369,7 @@
       <c r="B58">
         <v>2015</v>
       </c>
-      <c r="C58" s="74">
+      <c r="C58" s="73">
         <f t="shared" si="0"/>
         <v>42248</v>
       </c>
@@ -9237,7 +9393,7 @@
       <c r="B59">
         <v>2015</v>
       </c>
-      <c r="C59" s="74">
+      <c r="C59" s="73">
         <f t="shared" si="0"/>
         <v>42278</v>
       </c>
@@ -9261,7 +9417,7 @@
       <c r="B60">
         <v>2015</v>
       </c>
-      <c r="C60" s="74">
+      <c r="C60" s="73">
         <f t="shared" si="0"/>
         <v>42309</v>
       </c>
@@ -9285,7 +9441,7 @@
       <c r="B61">
         <v>2015</v>
       </c>
-      <c r="C61" s="74">
+      <c r="C61" s="73">
         <f t="shared" si="0"/>
         <v>42339</v>
       </c>
@@ -9309,7 +9465,7 @@
       <c r="B62">
         <v>2016</v>
       </c>
-      <c r="C62" s="74">
+      <c r="C62" s="73">
         <f t="shared" si="0"/>
         <v>42370</v>
       </c>
@@ -9333,7 +9489,7 @@
       <c r="B63">
         <v>2016</v>
       </c>
-      <c r="C63" s="74">
+      <c r="C63" s="73">
         <f t="shared" si="0"/>
         <v>42401</v>
       </c>
@@ -9357,7 +9513,7 @@
       <c r="B64">
         <v>2016</v>
       </c>
-      <c r="C64" s="74">
+      <c r="C64" s="73">
         <f t="shared" si="0"/>
         <v>42430</v>
       </c>
@@ -9381,7 +9537,7 @@
       <c r="B65">
         <v>2016</v>
       </c>
-      <c r="C65" s="74">
+      <c r="C65" s="73">
         <f t="shared" si="0"/>
         <v>42461</v>
       </c>
@@ -9405,7 +9561,7 @@
       <c r="B66">
         <v>2016</v>
       </c>
-      <c r="C66" s="74">
+      <c r="C66" s="73">
         <f t="shared" si="0"/>
         <v>42491</v>
       </c>
@@ -9429,7 +9585,7 @@
       <c r="B67">
         <v>2016</v>
       </c>
-      <c r="C67" s="74">
+      <c r="C67" s="73">
         <f t="shared" ref="C67:C109" si="1">DATE(B67,A67,1)</f>
         <v>42522</v>
       </c>
@@ -9453,7 +9609,7 @@
       <c r="B68">
         <v>2016</v>
       </c>
-      <c r="C68" s="74">
+      <c r="C68" s="73">
         <f t="shared" si="1"/>
         <v>42552</v>
       </c>
@@ -9477,7 +9633,7 @@
       <c r="B69">
         <v>2016</v>
       </c>
-      <c r="C69" s="74">
+      <c r="C69" s="73">
         <f t="shared" si="1"/>
         <v>42583</v>
       </c>
@@ -9501,7 +9657,7 @@
       <c r="B70">
         <v>2016</v>
       </c>
-      <c r="C70" s="74">
+      <c r="C70" s="73">
         <f t="shared" si="1"/>
         <v>42614</v>
       </c>
@@ -9525,7 +9681,7 @@
       <c r="B71">
         <v>2016</v>
       </c>
-      <c r="C71" s="74">
+      <c r="C71" s="73">
         <f t="shared" si="1"/>
         <v>42644</v>
       </c>
@@ -9549,7 +9705,7 @@
       <c r="B72">
         <v>2016</v>
       </c>
-      <c r="C72" s="74">
+      <c r="C72" s="73">
         <f t="shared" si="1"/>
         <v>42675</v>
       </c>
@@ -9573,7 +9729,7 @@
       <c r="B73">
         <v>2016</v>
       </c>
-      <c r="C73" s="74">
+      <c r="C73" s="73">
         <f t="shared" si="1"/>
         <v>42705</v>
       </c>
@@ -9597,7 +9753,7 @@
       <c r="B74">
         <v>2017</v>
       </c>
-      <c r="C74" s="74">
+      <c r="C74" s="73">
         <f t="shared" si="1"/>
         <v>42736</v>
       </c>
@@ -9621,7 +9777,7 @@
       <c r="B75">
         <v>2017</v>
       </c>
-      <c r="C75" s="74">
+      <c r="C75" s="73">
         <f t="shared" si="1"/>
         <v>42767</v>
       </c>
@@ -9645,7 +9801,7 @@
       <c r="B76">
         <v>2017</v>
       </c>
-      <c r="C76" s="74">
+      <c r="C76" s="73">
         <f t="shared" si="1"/>
         <v>42795</v>
       </c>
@@ -9669,7 +9825,7 @@
       <c r="B77">
         <v>2017</v>
       </c>
-      <c r="C77" s="74">
+      <c r="C77" s="73">
         <f t="shared" si="1"/>
         <v>42826</v>
       </c>
@@ -9693,7 +9849,7 @@
       <c r="B78">
         <v>2017</v>
       </c>
-      <c r="C78" s="74">
+      <c r="C78" s="73">
         <f t="shared" si="1"/>
         <v>42856</v>
       </c>
@@ -9717,7 +9873,7 @@
       <c r="B79">
         <v>2017</v>
       </c>
-      <c r="C79" s="74">
+      <c r="C79" s="73">
         <f t="shared" si="1"/>
         <v>42887</v>
       </c>
@@ -9741,7 +9897,7 @@
       <c r="B80">
         <v>2017</v>
       </c>
-      <c r="C80" s="74">
+      <c r="C80" s="73">
         <f t="shared" si="1"/>
         <v>42917</v>
       </c>
@@ -9765,7 +9921,7 @@
       <c r="B81">
         <v>2017</v>
       </c>
-      <c r="C81" s="74">
+      <c r="C81" s="73">
         <f t="shared" si="1"/>
         <v>42948</v>
       </c>
@@ -9789,7 +9945,7 @@
       <c r="B82">
         <v>2017</v>
       </c>
-      <c r="C82" s="74">
+      <c r="C82" s="73">
         <f t="shared" si="1"/>
         <v>42979</v>
       </c>
@@ -9813,7 +9969,7 @@
       <c r="B83">
         <v>2017</v>
       </c>
-      <c r="C83" s="74">
+      <c r="C83" s="73">
         <f t="shared" si="1"/>
         <v>43009</v>
       </c>
@@ -9837,7 +9993,7 @@
       <c r="B84">
         <v>2017</v>
       </c>
-      <c r="C84" s="74">
+      <c r="C84" s="73">
         <f t="shared" si="1"/>
         <v>43040</v>
       </c>
@@ -9861,7 +10017,7 @@
       <c r="B85">
         <v>2017</v>
       </c>
-      <c r="C85" s="74">
+      <c r="C85" s="73">
         <f t="shared" si="1"/>
         <v>43070</v>
       </c>
@@ -9885,7 +10041,7 @@
       <c r="B86">
         <v>2018</v>
       </c>
-      <c r="C86" s="74">
+      <c r="C86" s="73">
         <f t="shared" si="1"/>
         <v>43101</v>
       </c>
@@ -9909,7 +10065,7 @@
       <c r="B87">
         <v>2018</v>
       </c>
-      <c r="C87" s="74">
+      <c r="C87" s="73">
         <f t="shared" si="1"/>
         <v>43132</v>
       </c>
@@ -9933,7 +10089,7 @@
       <c r="B88">
         <v>2018</v>
       </c>
-      <c r="C88" s="74">
+      <c r="C88" s="73">
         <f t="shared" si="1"/>
         <v>43160</v>
       </c>
@@ -9957,7 +10113,7 @@
       <c r="B89">
         <v>2018</v>
       </c>
-      <c r="C89" s="74">
+      <c r="C89" s="73">
         <f t="shared" si="1"/>
         <v>43191</v>
       </c>
@@ -9981,7 +10137,7 @@
       <c r="B90">
         <v>2018</v>
       </c>
-      <c r="C90" s="74">
+      <c r="C90" s="73">
         <f t="shared" si="1"/>
         <v>43221</v>
       </c>
@@ -10005,7 +10161,7 @@
       <c r="B91">
         <v>2018</v>
       </c>
-      <c r="C91" s="74">
+      <c r="C91" s="73">
         <f t="shared" si="1"/>
         <v>43252</v>
       </c>
@@ -10029,7 +10185,7 @@
       <c r="B92">
         <v>2018</v>
       </c>
-      <c r="C92" s="74">
+      <c r="C92" s="73">
         <f t="shared" si="1"/>
         <v>43282</v>
       </c>
@@ -10053,7 +10209,7 @@
       <c r="B93">
         <v>2018</v>
       </c>
-      <c r="C93" s="74">
+      <c r="C93" s="73">
         <f t="shared" si="1"/>
         <v>43313</v>
       </c>
@@ -10077,7 +10233,7 @@
       <c r="B94">
         <v>2018</v>
       </c>
-      <c r="C94" s="74">
+      <c r="C94" s="73">
         <f t="shared" si="1"/>
         <v>43344</v>
       </c>
@@ -10101,7 +10257,7 @@
       <c r="B95">
         <v>2018</v>
       </c>
-      <c r="C95" s="74">
+      <c r="C95" s="73">
         <f t="shared" si="1"/>
         <v>43374</v>
       </c>
@@ -10125,7 +10281,7 @@
       <c r="B96">
         <v>2018</v>
       </c>
-      <c r="C96" s="74">
+      <c r="C96" s="73">
         <f t="shared" si="1"/>
         <v>43405</v>
       </c>
@@ -10149,7 +10305,7 @@
       <c r="B97">
         <v>2018</v>
       </c>
-      <c r="C97" s="74">
+      <c r="C97" s="73">
         <f t="shared" si="1"/>
         <v>43435</v>
       </c>
@@ -10173,7 +10329,7 @@
       <c r="B98">
         <v>2019</v>
       </c>
-      <c r="C98" s="74">
+      <c r="C98" s="73">
         <f t="shared" si="1"/>
         <v>43466</v>
       </c>
@@ -10197,7 +10353,7 @@
       <c r="B99">
         <v>2019</v>
       </c>
-      <c r="C99" s="74">
+      <c r="C99" s="73">
         <f t="shared" si="1"/>
         <v>43497</v>
       </c>
@@ -10221,7 +10377,7 @@
       <c r="B100">
         <v>2019</v>
       </c>
-      <c r="C100" s="74">
+      <c r="C100" s="73">
         <f t="shared" si="1"/>
         <v>43525</v>
       </c>
@@ -10245,7 +10401,7 @@
       <c r="B101">
         <v>2019</v>
       </c>
-      <c r="C101" s="74">
+      <c r="C101" s="73">
         <f t="shared" si="1"/>
         <v>43556</v>
       </c>
@@ -10269,7 +10425,7 @@
       <c r="B102">
         <v>2019</v>
       </c>
-      <c r="C102" s="74">
+      <c r="C102" s="73">
         <f t="shared" si="1"/>
         <v>43586</v>
       </c>
@@ -10293,7 +10449,7 @@
       <c r="B103">
         <v>2019</v>
       </c>
-      <c r="C103" s="74">
+      <c r="C103" s="73">
         <f t="shared" si="1"/>
         <v>43617</v>
       </c>
@@ -10317,7 +10473,7 @@
       <c r="B104">
         <v>2019</v>
       </c>
-      <c r="C104" s="74">
+      <c r="C104" s="73">
         <f t="shared" si="1"/>
         <v>43647</v>
       </c>
@@ -10341,7 +10497,7 @@
       <c r="B105">
         <v>2019</v>
       </c>
-      <c r="C105" s="74">
+      <c r="C105" s="73">
         <f t="shared" si="1"/>
         <v>43678</v>
       </c>
@@ -10365,7 +10521,7 @@
       <c r="B106">
         <v>2019</v>
       </c>
-      <c r="C106" s="74">
+      <c r="C106" s="73">
         <f t="shared" si="1"/>
         <v>43709</v>
       </c>
@@ -10389,7 +10545,7 @@
       <c r="B107">
         <v>2019</v>
       </c>
-      <c r="C107" s="74">
+      <c r="C107" s="73">
         <f t="shared" si="1"/>
         <v>43739</v>
       </c>
@@ -10413,7 +10569,7 @@
       <c r="B108">
         <v>2019</v>
       </c>
-      <c r="C108" s="74">
+      <c r="C108" s="73">
         <f t="shared" si="1"/>
         <v>43770</v>
       </c>
@@ -10437,7 +10593,7 @@
       <c r="B109">
         <v>2019</v>
       </c>
-      <c r="C109" s="74">
+      <c r="C109" s="73">
         <f t="shared" si="1"/>
         <v>43800</v>
       </c>
@@ -10461,229 +10617,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5564981C-E4C1-4223-BBB8-B7B238FE5FB5}">
-  <dimension ref="B2:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="29">
-        <f>LCA_Daily!D3</f>
-        <v>0.38667477943413398</v>
-      </c>
-      <c r="D3" s="28">
-        <v>600</v>
-      </c>
-      <c r="E3" s="27">
-        <v>85</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="33">
-        <f>C3*(1-(E3/D3))+(E3/D3)</f>
-        <v>0.47356251901429836</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="29">
-        <f>LCA_Daily!D4</f>
-        <v>0.470946151505932</v>
-      </c>
-      <c r="D4" s="28">
-        <v>460</v>
-      </c>
-      <c r="E4" s="27">
-        <v>85</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="33">
-        <f>C4*(1-(E4/D4))+(E4/D4)</f>
-        <v>0.56870610177114023</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="29">
-        <f>LCA_Daily!D5</f>
-        <v>0.52327350167325803</v>
-      </c>
-      <c r="D5" s="28">
-        <v>405</v>
-      </c>
-      <c r="E5" s="27">
-        <v>85</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="33">
-        <f>C5*(1-(E5/D5))+(E5/D5)</f>
-        <v>0.62332721119862367</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="29">
-        <f>LCA_Daily!D6</f>
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="D6" s="28">
-        <v>942</v>
-      </c>
-      <c r="E6" s="27">
-        <v>0</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="33">
-        <f>C6*(1-(E6/D6))+(E6/D6)</f>
-        <v>0.20687557042896301</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="29">
-        <f>LCA_Daily!D7</f>
-        <v>0.20687557042896301</v>
-      </c>
-      <c r="D7" s="28">
-        <v>942</v>
-      </c>
-      <c r="E7" s="27">
-        <v>0</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="33">
-        <f>C7*(1-(E7/D7))+(E7/D7)</f>
-        <v>0.20687557042896301</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="72" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="73"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="13">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="15">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="73"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="13">
-        <f>C12*(22/24)</f>
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="13">
-        <f>C11-C17</f>
-        <v>0.16666666666666669</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="13">
-        <f>C11*(8/24)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="15">
-        <f>C12-C15</f>
-        <v>6.25E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B10:C10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13276EEC-9828-43A0-B1C3-364F0B6ECE82}">
   <dimension ref="A1:N722"/>
   <sheetViews>

</xml_diff>

<commit_message>
modifications for new gas prices. tbh a bit messy. averaged out category in output prices
</commit_message>
<xml_diff>
--- a/data/LCA.xlsx
+++ b/data/LCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnergyDevelopment_Policy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EC218D-85D7-4D9B-B245-64E188626E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52578DDB-3665-46FB-8BC2-A0B47BCC9579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4650" windowWidth="29040" windowHeight="15840" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DB39A55B-965A-4C48-890F-EBD6380D77B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="6" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Graphing!$A$2:$N$424</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="71">
   <si>
     <t>Turbine</t>
   </si>
@@ -249,9 +250,6 @@
     <t>NG_Price</t>
   </si>
   <si>
-    <t>Raw CF Daily</t>
-  </si>
-  <si>
     <t>Raw CF Hourly</t>
   </si>
   <si>
@@ -263,8 +261,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="[$-409]mmm\-yy;@"/>
-    <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -515,13 +513,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -533,11 +525,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5719,10 +5717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B724EB-6910-45D9-ADF5-6C5EE28B5832}">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,36 +5728,37 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="7" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="15" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="V1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>50</v>
       </c>
@@ -5775,11 +5774,11 @@
       <c r="E2" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>71</v>
+      <c r="G2" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="H2" s="27" t="s">
         <v>19</v>
@@ -5814,23 +5813,20 @@
       <c r="R2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="32" t="s">
+      <c r="S2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="32" t="s">
+      <c r="T2" s="30" t="s">
         <v>12</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="V2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="27"/>
@@ -5879,23 +5875,20 @@
       <c r="R3" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="S3" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" s="39" t="s">
+      <c r="S3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="39" t="s">
+      <c r="T3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="39" t="s">
+      <c r="U3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="39" t="s">
+      <c r="V3" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -5905,12 +5898,12 @@
       <c r="C4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="29">
         <v>0.39965009698398801</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="31">
         <f>'CF Adjustment'!I3</f>
-        <v>0.48469966657792307</v>
+        <v>0.48469966657792302</v>
       </c>
       <c r="F4" s="25">
         <v>6800</v>
@@ -5926,22 +5919,22 @@
       <c r="J4">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="35">
         <f>J4*G4/(10^3)</f>
         <v>0.17054400000000003</v>
       </c>
-      <c r="L4" s="37">
+      <c r="L4" s="35">
         <f>K4*H4*8670*E4/2000</f>
-        <v>215.00547445578673</v>
+        <v>215.0054744557867</v>
       </c>
       <c r="M4">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="34">
         <f>M4*G4/(10^3)</f>
         <v>5.5352000000000005E-3</v>
       </c>
-      <c r="O4" s="37">
+      <c r="O4" s="35">
         <f>N4*H4*8670*E4/2000</f>
         <v>6.9782478551439544</v>
       </c>
@@ -5952,27 +5945,26 @@
         <f>P4*G4/(10^3)</f>
         <v>875.16000000000008</v>
       </c>
-      <c r="R4" s="38">
+      <c r="R4" s="36">
         <f>Q4*H4*8670*E4/2000</f>
         <v>1103317.5662862738</v>
       </c>
-      <c r="S4" s="23"/>
-      <c r="T4" s="5">
+      <c r="S4" s="5">
         <v>200</v>
       </c>
-      <c r="U4" s="38">
-        <f>$E4*8760*$T4*H4/10^6</f>
-        <v>509.51628950671278</v>
-      </c>
-      <c r="V4" s="5">
+      <c r="T4" s="36">
+        <f>$E4*8760*$S4*H4/10^6</f>
+        <v>509.51628950671267</v>
+      </c>
+      <c r="U4" s="5">
         <v>250</v>
       </c>
-      <c r="W4" s="38">
-        <f>$E4*8760*$V4*H4/10^6</f>
-        <v>636.89536188339105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="V4" s="36">
+        <f>$E4*8760*$U4*H4/10^6</f>
+        <v>636.89536188339082</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -5982,10 +5974,10 @@
       <c r="C5" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <v>0.50860178247690002</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="31">
         <f>'CF Adjustment'!I4</f>
         <v>0.59940362701921202</v>
       </c>
@@ -5993,7 +5985,7 @@
         <v>6400</v>
       </c>
       <c r="G5" s="25">
-        <f t="shared" ref="G5:G8" si="0">F5*1.1</f>
+        <f>F5*1.1</f>
         <v>7040.0000000000009</v>
       </c>
       <c r="H5" s="23">
@@ -6003,23 +5995,23 @@
       <c r="J5">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="35">
         <f>J5*G5/(10^3)</f>
         <v>0.16051200000000002</v>
       </c>
-      <c r="L5" s="37">
+      <c r="L5" s="35">
         <f>K5*H5*8670*E5/2000</f>
         <v>191.8553022578329</v>
       </c>
       <c r="M5">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="N5" s="36">
+      <c r="N5" s="34">
         <f>M5*G5/(10^3)</f>
         <v>5.2096000000000009E-3</v>
       </c>
-      <c r="O5" s="37">
-        <f t="shared" ref="O5:O8" si="1">N5*H5*8670*E5/2000</f>
+      <c r="O5" s="35">
+        <f>N5*H5*8670*E5/2000</f>
         <v>6.2268826171401903</v>
       </c>
       <c r="P5" s="5">
@@ -6029,27 +6021,26 @@
         <f>P5*G5/(10^3)</f>
         <v>823.68000000000006</v>
       </c>
-      <c r="R5" s="38">
+      <c r="R5" s="36">
         <f>Q5*H5*8670*E5/2000</f>
         <v>984520.63000730053</v>
       </c>
-      <c r="S5" s="23"/>
-      <c r="T5" s="5">
+      <c r="S5" s="5">
         <v>200</v>
       </c>
-      <c r="U5" s="38">
-        <f>$E5*8760*$T5*H5/10^6</f>
+      <c r="T5" s="36">
+        <f>$E5*8760*$S5*H5/10^6</f>
         <v>483.07137108732331</v>
       </c>
-      <c r="V5" s="5">
+      <c r="U5" s="5">
         <v>250</v>
       </c>
-      <c r="W5" s="38">
-        <f t="shared" ref="W5:W8" si="2">$E5*8760*$V5*H5/10^6</f>
+      <c r="V5" s="36">
+        <f>$E5*8760*$U5*H5/10^6</f>
         <v>603.83921385915426</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -6059,10 +6050,10 @@
       <c r="C6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>0.57685822589000002</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="31">
         <f>'CF Adjustment'!I5</f>
         <v>0.66566575872790124</v>
       </c>
@@ -6070,7 +6061,7 @@
         <v>6200</v>
       </c>
       <c r="G6" s="25">
-        <f t="shared" si="0"/>
+        <f>F6*1.1</f>
         <v>6820.0000000000009</v>
       </c>
       <c r="H6" s="23">
@@ -6080,53 +6071,52 @@
       <c r="J6">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="K6" s="37">
-        <f t="shared" ref="K5:K8" si="3">J6*G6/(10^3)</f>
+      <c r="K6" s="35">
+        <f>J6*G6/(10^3)</f>
         <v>0.15549600000000005</v>
       </c>
-      <c r="L6" s="37">
-        <f t="shared" ref="L5:L12" si="4">K6*H6*8670*E6/2000</f>
+      <c r="L6" s="35">
+        <f t="shared" ref="L6:L12" si="0">K6*H6*8670*E6/2000</f>
         <v>181.72704489251777</v>
       </c>
       <c r="M6">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="N6" s="36">
-        <f t="shared" ref="N5:N8" si="5">M6*G6/(10^3)</f>
+      <c r="N6" s="34">
+        <f>M6*G6/(10^3)</f>
         <v>5.0468000000000006E-3</v>
       </c>
-      <c r="O6" s="37">
-        <f t="shared" si="1"/>
+      <c r="O6" s="35">
+        <f>N6*H6*8670*E6/2000</f>
         <v>5.8981584745817166</v>
       </c>
       <c r="P6" s="5">
         <v>117</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q5:Q8" si="6">P6*G6/(10^3)</f>
+        <f>P6*G6/(10^3)</f>
         <v>797.94000000000017</v>
       </c>
-      <c r="R6" s="38">
-        <f t="shared" ref="R5:R8" si="7">Q6*H6*8670*E6/2000</f>
+      <c r="R6" s="36">
+        <f>Q6*H6*8670*E6/2000</f>
         <v>932546.67773792008</v>
       </c>
-      <c r="S6" s="23"/>
-      <c r="T6" s="5">
+      <c r="S6" s="5">
         <v>200</v>
       </c>
-      <c r="U6" s="38">
-        <f t="shared" ref="U5:U8" si="8">$E6*8760*$T6*H6/10^6</f>
+      <c r="T6" s="36">
+        <f>$E6*8760*$S6*H6/10^6</f>
         <v>472.32979576296964</v>
       </c>
-      <c r="V6" s="5">
+      <c r="U6" s="5">
         <v>250</v>
       </c>
-      <c r="W6" s="38">
-        <f t="shared" si="2"/>
+      <c r="V6" s="36">
+        <f>$E6*8760*$U6*H6/10^6</f>
         <v>590.41224470371196</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>48</v>
       </c>
@@ -6136,10 +6126,10 @@
       <c r="C7" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>0.39456636113540999</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="31">
         <f>'CF Adjustment'!I6</f>
         <v>0.39456636113540999</v>
       </c>
@@ -6147,7 +6137,7 @@
         <v>7760</v>
       </c>
       <c r="G7" s="25">
-        <f t="shared" si="0"/>
+        <f>F7*1.1</f>
         <v>8536</v>
       </c>
       <c r="H7" s="23">
@@ -6157,53 +6147,52 @@
       <c r="J7">
         <v>0.15</v>
       </c>
-      <c r="K7" s="37">
-        <f t="shared" si="3"/>
+      <c r="K7" s="35">
+        <f>J7*G7/(10^3)</f>
         <v>1.2803999999999998</v>
       </c>
-      <c r="L7" s="37">
-        <f t="shared" si="4"/>
+      <c r="L7" s="35">
+        <f t="shared" si="0"/>
         <v>2063.030870579546</v>
       </c>
       <c r="M7">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="N7" s="36">
-        <f t="shared" si="5"/>
+      <c r="N7" s="34">
+        <f>M7*G7/(10^3)</f>
         <v>6.3166399999999992E-3</v>
       </c>
-      <c r="O7" s="37">
-        <f t="shared" si="1"/>
+      <c r="O7" s="35">
+        <f>N7*H7*8670*E7/2000</f>
         <v>10.177618961525761</v>
       </c>
       <c r="P7" s="5">
         <v>117</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="6"/>
+        <f>P7*G7/(10^3)</f>
         <v>998.71199999999999</v>
       </c>
-      <c r="R7" s="38">
-        <f t="shared" si="7"/>
+      <c r="R7" s="36">
+        <f>Q7*H7*8670*E7/2000</f>
         <v>1609164.0790520462</v>
       </c>
-      <c r="S7" s="23"/>
-      <c r="T7" s="5">
+      <c r="S7" s="5">
         <v>200</v>
       </c>
-      <c r="U7" s="38">
-        <f t="shared" si="8"/>
+      <c r="T7" s="36">
+        <f>$E7*8760*$S7*H7/10^6</f>
         <v>651.18600935610243</v>
       </c>
-      <c r="V7" s="5">
+      <c r="U7" s="5">
         <v>250</v>
       </c>
-      <c r="W7" s="38">
-        <f t="shared" si="2"/>
+      <c r="V7" s="36">
+        <f>$E7*8760*$U7*H7/10^6</f>
         <v>813.9825116951281</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -6213,10 +6202,10 @@
       <c r="C8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>0.39456636113540999</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="31">
         <f>'CF Adjustment'!I7</f>
         <v>0.39456636113540999</v>
       </c>
@@ -6224,7 +6213,7 @@
         <v>7760</v>
       </c>
       <c r="G8" s="25">
-        <f t="shared" si="0"/>
+        <f>F8*1.1</f>
         <v>8536</v>
       </c>
       <c r="H8" s="23">
@@ -6234,54 +6223,53 @@
       <c r="J8">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="K8" s="37">
-        <f t="shared" si="3"/>
+      <c r="K8" s="35">
+        <f>J8*G8/(10^3)</f>
         <v>0.19462080000000001</v>
       </c>
-      <c r="L8" s="37">
-        <f t="shared" si="4"/>
+      <c r="L8" s="35">
+        <f t="shared" si="0"/>
         <v>313.580692328091</v>
       </c>
       <c r="M8">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="N8" s="36">
-        <f t="shared" si="5"/>
+      <c r="N8" s="34">
+        <f>M8*G8/(10^3)</f>
         <v>6.3166399999999992E-3</v>
       </c>
-      <c r="O8" s="37">
-        <f t="shared" si="1"/>
+      <c r="O8" s="35">
+        <f>N8*H8*8670*E8/2000</f>
         <v>10.177618961525761</v>
       </c>
       <c r="P8" s="5">
         <v>117</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f>P8*G8/(10^3)</f>
         <v>998.71199999999999</v>
       </c>
-      <c r="R8" s="38">
-        <f t="shared" si="7"/>
+      <c r="R8" s="36">
+        <f>Q8*H8*8670*E8/2000</f>
         <v>1609164.0790520462</v>
       </c>
-      <c r="S8" s="23"/>
-      <c r="T8" s="5">
+      <c r="S8" s="5">
         <v>200</v>
       </c>
-      <c r="U8" s="38">
-        <f t="shared" si="8"/>
+      <c r="T8" s="36">
+        <f>$E8*8760*$S8*H8/10^6</f>
         <v>651.18600935610243</v>
       </c>
-      <c r="V8" s="5">
+      <c r="U8" s="5">
         <v>250</v>
       </c>
-      <c r="W8" s="38">
-        <f t="shared" si="2"/>
+      <c r="V8" s="36">
+        <f>$E8*8760*$U8*H8/10^6</f>
         <v>813.9825116951281</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -6290,7 +6278,7 @@
       <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <f>'CF Adjustment'!C12*0.203+'CF Adjustment'!C11*0.702</f>
         <v>0.32774999999999999</v>
       </c>
@@ -6305,26 +6293,23 @@
         <v>8000</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K5:K12" si="9">J9*F9/(10^3)</f>
+        <f t="shared" ref="K9:K12" si="1">J9*F9/(10^3)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q9">
         <v>55</v>
       </c>
-      <c r="R9" s="37">
+      <c r="R9" s="35">
         <f>E9*Q9*8760*H9/(10^6)</f>
         <v>39.477487499999995</v>
       </c>
-      <c r="S9" s="23">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+    </row>
+    <row r="10" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -6333,12 +6318,12 @@
       <c r="C10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <f>0.53*'CF Adjustment'!C15+0.342*'CF Adjustment'!C16+0.49*'CF Adjustment'!C17+0.53*'CF Adjustment'!C18</f>
         <v>0.49533333333333335</v>
       </c>
       <c r="E10" s="24">
-        <f t="shared" ref="E10:E12" si="10">D10</f>
+        <f>D10</f>
         <v>0.49533333333333335</v>
       </c>
       <c r="H10">
@@ -6348,26 +6333,23 @@
         <v>38000</v>
       </c>
       <c r="K10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q10">
         <v>13</v>
       </c>
-      <c r="R10" s="37">
-        <f t="shared" ref="R10:R12" si="11">E10*Q10*8760*H10/(10^6)</f>
+      <c r="R10" s="35">
+        <f>E10*Q10*8760*H10/(10^6)</f>
         <v>14.102140000000002</v>
       </c>
-      <c r="S10" s="23">
-        <v>38000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -6376,12 +6358,12 @@
       <c r="C11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="29">
         <f>0.498*'CF Adjustment'!C12+0.435*'CF Adjustment'!C16+0.456*'CF Adjustment'!C17</f>
         <v>0.48399999999999999</v>
       </c>
       <c r="E11" s="24">
-        <f t="shared" si="10"/>
+        <f>D11</f>
         <v>0.48399999999999999</v>
       </c>
       <c r="H11">
@@ -6391,26 +6373,23 @@
         <v>20000</v>
       </c>
       <c r="K11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q11">
         <v>13</v>
       </c>
-      <c r="R11" s="37">
-        <f t="shared" si="11"/>
+      <c r="R11" s="35">
+        <f>E11*Q11*8760*H11/(10^6)</f>
         <v>11.023584</v>
       </c>
-      <c r="S11" s="23">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -6419,12 +6398,12 @@
       <c r="C12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="29">
         <f>0.454*'CF Adjustment'!C12+0.419*'CF Adjustment'!C16+0.428*'CF Adjustment'!C17</f>
         <v>0.44600000000000006</v>
       </c>
       <c r="E12" s="24">
-        <f t="shared" si="10"/>
+        <f>D12</f>
         <v>0.44600000000000006</v>
       </c>
       <c r="H12">
@@ -6434,35 +6413,30 @@
         <v>20000</v>
       </c>
       <c r="K12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q12">
         <v>13</v>
       </c>
-      <c r="R12" s="37">
-        <f t="shared" si="11"/>
+      <c r="R12" s="35">
+        <f>E12*Q12*8760*H12/(10^6)</f>
         <v>7.6185720000000021</v>
       </c>
-      <c r="S12" s="23">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D13" s="23"/>
       <c r="I13" s="23"/>
-      <c r="S13" s="23"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I14" s="23"/>
-      <c r="S14" s="23"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="T15" t="s">
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6476,8 +6450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5564981C-E4C1-4223-BBB8-B7B238FE5FB5}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6494,11 +6468,9 @@
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>44</v>
@@ -6520,10 +6492,7 @@
       <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15">
-        <f>LCA!D4</f>
-        <v>0.39965009698398801</v>
-      </c>
+      <c r="C3" s="15"/>
       <c r="D3" s="15">
         <f>LCA!D4</f>
         <v>0.39965009698398801</v>
@@ -6537,23 +6506,17 @@
       <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="19">
-        <f>C3*(1-(F3/E3))+(F3/E3)</f>
-        <v>0.48469966657792307</v>
-      </c>
+      <c r="H3" s="19"/>
       <c r="I3" s="19">
-        <f>D3*(1-(F3/E3))+(F3/E3)</f>
-        <v>0.48469966657792307</v>
+        <f>F3/E3+(E3-F3)*D3/E3</f>
+        <v>0.48469966657792302</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="15">
-        <f>LCA!D5</f>
-        <v>0.50860178247690002</v>
-      </c>
+      <c r="C4" s="15"/>
       <c r="D4" s="15">
         <f>LCA!D5</f>
         <v>0.50860178247690002</v>
@@ -6567,12 +6530,9 @@
       <c r="G4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="19">
-        <f>C4*(1-(F4/E4))+(F4/E4)</f>
-        <v>0.59940362701921202</v>
-      </c>
+      <c r="H4" s="19"/>
       <c r="I4" s="19">
-        <f t="shared" ref="I4:I7" si="0">D4*(1-(F4/E4))+(F4/E4)</f>
+        <f t="shared" ref="I4:I7" si="0">F4/E4+(E4-F4)*D4/E4</f>
         <v>0.59940362701921202</v>
       </c>
     </row>
@@ -6580,10 +6540,7 @@
       <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15">
-        <f>LCA!D6</f>
-        <v>0.57685822589000002</v>
-      </c>
+      <c r="C5" s="15"/>
       <c r="D5" s="15">
         <f>LCA!D6</f>
         <v>0.57685822589000002</v>
@@ -6597,10 +6554,7 @@
       <c r="G5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="19">
-        <f>C5*(1-(F5/E5))+(F5/E5)</f>
-        <v>0.66566575872790124</v>
-      </c>
+      <c r="H5" s="19"/>
       <c r="I5" s="19">
         <f t="shared" si="0"/>
         <v>0.66566575872790124</v>
@@ -6610,10 +6564,7 @@
       <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="15">
-        <f>LCA!D7</f>
-        <v>0.39456636113540999</v>
-      </c>
+      <c r="C6" s="15"/>
       <c r="D6" s="15">
         <f>LCA!D7</f>
         <v>0.39456636113540999</v>
@@ -6627,10 +6578,7 @@
       <c r="G6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="19">
-        <f>C6*(1-(F6/E6))+(F6/E6)</f>
-        <v>0.39456636113540999</v>
-      </c>
+      <c r="H6" s="19"/>
       <c r="I6" s="19">
         <f t="shared" si="0"/>
         <v>0.39456636113540999</v>
@@ -6640,10 +6588,7 @@
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
-        <f>LCA!D8</f>
-        <v>0.39456636113540999</v>
-      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="15">
         <f>LCA!D8</f>
         <v>0.39456636113540999</v>
@@ -6657,10 +6602,7 @@
       <c r="G7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="19">
-        <f>C7*(1-(F7/E7))+(F7/E7)</f>
-        <v>0.39456636113540999</v>
-      </c>
+      <c r="H7" s="19"/>
       <c r="I7" s="19">
         <f t="shared" si="0"/>
         <v>0.39456636113540999</v>
@@ -6668,11 +6610,11 @@
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="34"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="32"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -6694,11 +6636,11 @@
     </row>
     <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="34"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -6790,7 +6732,7 @@
       <c r="B2">
         <v>2011</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="28">
         <f>DATE(B2,A2,1)</f>
         <v>40544</v>
       </c>
@@ -6814,7 +6756,7 @@
       <c r="B3">
         <v>2011</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="28">
         <f t="shared" ref="C3:C66" si="0">DATE(B3,A3,1)</f>
         <v>40575</v>
       </c>
@@ -6838,7 +6780,7 @@
       <c r="B4">
         <v>2011</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <f t="shared" si="0"/>
         <v>40603</v>
       </c>
@@ -6862,7 +6804,7 @@
       <c r="B5">
         <v>2011</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="28">
         <f t="shared" si="0"/>
         <v>40634</v>
       </c>
@@ -6886,7 +6828,7 @@
       <c r="B6">
         <v>2011</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="28">
         <f t="shared" si="0"/>
         <v>40664</v>
       </c>
@@ -6910,7 +6852,7 @@
       <c r="B7">
         <v>2011</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <f t="shared" si="0"/>
         <v>40695</v>
       </c>
@@ -6934,7 +6876,7 @@
       <c r="B8">
         <v>2011</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="28">
         <f t="shared" si="0"/>
         <v>40725</v>
       </c>
@@ -6958,7 +6900,7 @@
       <c r="B9">
         <v>2011</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <f t="shared" si="0"/>
         <v>40756</v>
       </c>
@@ -6982,7 +6924,7 @@
       <c r="B10">
         <v>2011</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="28">
         <f t="shared" si="0"/>
         <v>40787</v>
       </c>
@@ -7006,7 +6948,7 @@
       <c r="B11">
         <v>2011</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="28">
         <f t="shared" si="0"/>
         <v>40817</v>
       </c>
@@ -7030,7 +6972,7 @@
       <c r="B12">
         <v>2011</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="28">
         <f t="shared" si="0"/>
         <v>40848</v>
       </c>
@@ -7054,7 +6996,7 @@
       <c r="B13">
         <v>2011</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="28">
         <f t="shared" si="0"/>
         <v>40878</v>
       </c>
@@ -7078,7 +7020,7 @@
       <c r="B14">
         <v>2012</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="28">
         <f t="shared" si="0"/>
         <v>40909</v>
       </c>
@@ -7102,7 +7044,7 @@
       <c r="B15">
         <v>2012</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="28">
         <f t="shared" si="0"/>
         <v>40940</v>
       </c>
@@ -7126,7 +7068,7 @@
       <c r="B16">
         <v>2012</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="28">
         <f t="shared" si="0"/>
         <v>40969</v>
       </c>
@@ -7150,7 +7092,7 @@
       <c r="B17">
         <v>2012</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="28">
         <f t="shared" si="0"/>
         <v>41000</v>
       </c>
@@ -7174,7 +7116,7 @@
       <c r="B18">
         <v>2012</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="28">
         <f t="shared" si="0"/>
         <v>41030</v>
       </c>
@@ -7198,7 +7140,7 @@
       <c r="B19">
         <v>2012</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="28">
         <f t="shared" si="0"/>
         <v>41061</v>
       </c>
@@ -7222,7 +7164,7 @@
       <c r="B20">
         <v>2012</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="28">
         <f t="shared" si="0"/>
         <v>41091</v>
       </c>
@@ -7246,7 +7188,7 @@
       <c r="B21">
         <v>2012</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="28">
         <f t="shared" si="0"/>
         <v>41122</v>
       </c>
@@ -7270,7 +7212,7 @@
       <c r="B22">
         <v>2012</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="28">
         <f t="shared" si="0"/>
         <v>41153</v>
       </c>
@@ -7294,7 +7236,7 @@
       <c r="B23">
         <v>2012</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="28">
         <f t="shared" si="0"/>
         <v>41183</v>
       </c>
@@ -7318,7 +7260,7 @@
       <c r="B24">
         <v>2012</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="28">
         <f t="shared" si="0"/>
         <v>41214</v>
       </c>
@@ -7342,7 +7284,7 @@
       <c r="B25">
         <v>2012</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="28">
         <f t="shared" si="0"/>
         <v>41244</v>
       </c>
@@ -7366,7 +7308,7 @@
       <c r="B26">
         <v>2013</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="28">
         <f t="shared" si="0"/>
         <v>41275</v>
       </c>
@@ -7390,7 +7332,7 @@
       <c r="B27">
         <v>2013</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="28">
         <f t="shared" si="0"/>
         <v>41306</v>
       </c>
@@ -7414,7 +7356,7 @@
       <c r="B28">
         <v>2013</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="28">
         <f t="shared" si="0"/>
         <v>41334</v>
       </c>
@@ -7438,7 +7380,7 @@
       <c r="B29">
         <v>2013</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="28">
         <f t="shared" si="0"/>
         <v>41365</v>
       </c>
@@ -7462,7 +7404,7 @@
       <c r="B30">
         <v>2013</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="28">
         <f t="shared" si="0"/>
         <v>41395</v>
       </c>
@@ -7486,7 +7428,7 @@
       <c r="B31">
         <v>2013</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="28">
         <f t="shared" si="0"/>
         <v>41426</v>
       </c>
@@ -7510,7 +7452,7 @@
       <c r="B32">
         <v>2013</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C32" s="28">
         <f t="shared" si="0"/>
         <v>41456</v>
       </c>
@@ -7534,7 +7476,7 @@
       <c r="B33">
         <v>2013</v>
       </c>
-      <c r="C33" s="30">
+      <c r="C33" s="28">
         <f t="shared" si="0"/>
         <v>41487</v>
       </c>
@@ -7558,7 +7500,7 @@
       <c r="B34">
         <v>2013</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="28">
         <f t="shared" si="0"/>
         <v>41518</v>
       </c>
@@ -7582,7 +7524,7 @@
       <c r="B35">
         <v>2013</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C35" s="28">
         <f t="shared" si="0"/>
         <v>41548</v>
       </c>
@@ -7606,7 +7548,7 @@
       <c r="B36">
         <v>2013</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="28">
         <f t="shared" si="0"/>
         <v>41579</v>
       </c>
@@ -7630,7 +7572,7 @@
       <c r="B37">
         <v>2013</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="28">
         <f t="shared" si="0"/>
         <v>41609</v>
       </c>
@@ -7654,7 +7596,7 @@
       <c r="B38">
         <v>2014</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="28">
         <f t="shared" si="0"/>
         <v>41640</v>
       </c>
@@ -7678,7 +7620,7 @@
       <c r="B39">
         <v>2014</v>
       </c>
-      <c r="C39" s="30">
+      <c r="C39" s="28">
         <f t="shared" si="0"/>
         <v>41671</v>
       </c>
@@ -7702,7 +7644,7 @@
       <c r="B40">
         <v>2014</v>
       </c>
-      <c r="C40" s="30">
+      <c r="C40" s="28">
         <f t="shared" si="0"/>
         <v>41699</v>
       </c>
@@ -7726,7 +7668,7 @@
       <c r="B41">
         <v>2014</v>
       </c>
-      <c r="C41" s="30">
+      <c r="C41" s="28">
         <f t="shared" si="0"/>
         <v>41730</v>
       </c>
@@ -7750,7 +7692,7 @@
       <c r="B42">
         <v>2014</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C42" s="28">
         <f t="shared" si="0"/>
         <v>41760</v>
       </c>
@@ -7774,7 +7716,7 @@
       <c r="B43">
         <v>2014</v>
       </c>
-      <c r="C43" s="30">
+      <c r="C43" s="28">
         <f t="shared" si="0"/>
         <v>41791</v>
       </c>
@@ -7798,7 +7740,7 @@
       <c r="B44">
         <v>2014</v>
       </c>
-      <c r="C44" s="30">
+      <c r="C44" s="28">
         <f t="shared" si="0"/>
         <v>41821</v>
       </c>
@@ -7822,7 +7764,7 @@
       <c r="B45">
         <v>2014</v>
       </c>
-      <c r="C45" s="30">
+      <c r="C45" s="28">
         <f t="shared" si="0"/>
         <v>41852</v>
       </c>
@@ -7846,7 +7788,7 @@
       <c r="B46">
         <v>2014</v>
       </c>
-      <c r="C46" s="30">
+      <c r="C46" s="28">
         <f t="shared" si="0"/>
         <v>41883</v>
       </c>
@@ -7870,7 +7812,7 @@
       <c r="B47">
         <v>2014</v>
       </c>
-      <c r="C47" s="30">
+      <c r="C47" s="28">
         <f t="shared" si="0"/>
         <v>41913</v>
       </c>
@@ -7894,7 +7836,7 @@
       <c r="B48">
         <v>2014</v>
       </c>
-      <c r="C48" s="30">
+      <c r="C48" s="28">
         <f t="shared" si="0"/>
         <v>41944</v>
       </c>
@@ -7918,7 +7860,7 @@
       <c r="B49">
         <v>2014</v>
       </c>
-      <c r="C49" s="30">
+      <c r="C49" s="28">
         <f t="shared" si="0"/>
         <v>41974</v>
       </c>
@@ -7942,7 +7884,7 @@
       <c r="B50">
         <v>2015</v>
       </c>
-      <c r="C50" s="30">
+      <c r="C50" s="28">
         <f t="shared" si="0"/>
         <v>42005</v>
       </c>
@@ -7966,7 +7908,7 @@
       <c r="B51">
         <v>2015</v>
       </c>
-      <c r="C51" s="30">
+      <c r="C51" s="28">
         <f t="shared" si="0"/>
         <v>42036</v>
       </c>
@@ -7990,7 +7932,7 @@
       <c r="B52">
         <v>2015</v>
       </c>
-      <c r="C52" s="30">
+      <c r="C52" s="28">
         <f t="shared" si="0"/>
         <v>42064</v>
       </c>
@@ -8014,7 +7956,7 @@
       <c r="B53">
         <v>2015</v>
       </c>
-      <c r="C53" s="30">
+      <c r="C53" s="28">
         <f t="shared" si="0"/>
         <v>42095</v>
       </c>
@@ -8038,7 +7980,7 @@
       <c r="B54">
         <v>2015</v>
       </c>
-      <c r="C54" s="30">
+      <c r="C54" s="28">
         <f t="shared" si="0"/>
         <v>42125</v>
       </c>
@@ -8062,7 +8004,7 @@
       <c r="B55">
         <v>2015</v>
       </c>
-      <c r="C55" s="30">
+      <c r="C55" s="28">
         <f t="shared" si="0"/>
         <v>42156</v>
       </c>
@@ -8086,7 +8028,7 @@
       <c r="B56">
         <v>2015</v>
       </c>
-      <c r="C56" s="30">
+      <c r="C56" s="28">
         <f t="shared" si="0"/>
         <v>42186</v>
       </c>
@@ -8110,7 +8052,7 @@
       <c r="B57">
         <v>2015</v>
       </c>
-      <c r="C57" s="30">
+      <c r="C57" s="28">
         <f t="shared" si="0"/>
         <v>42217</v>
       </c>
@@ -8134,7 +8076,7 @@
       <c r="B58">
         <v>2015</v>
       </c>
-      <c r="C58" s="30">
+      <c r="C58" s="28">
         <f t="shared" si="0"/>
         <v>42248</v>
       </c>
@@ -8158,7 +8100,7 @@
       <c r="B59">
         <v>2015</v>
       </c>
-      <c r="C59" s="30">
+      <c r="C59" s="28">
         <f t="shared" si="0"/>
         <v>42278</v>
       </c>
@@ -8182,7 +8124,7 @@
       <c r="B60">
         <v>2015</v>
       </c>
-      <c r="C60" s="30">
+      <c r="C60" s="28">
         <f t="shared" si="0"/>
         <v>42309</v>
       </c>
@@ -8206,7 +8148,7 @@
       <c r="B61">
         <v>2015</v>
       </c>
-      <c r="C61" s="30">
+      <c r="C61" s="28">
         <f t="shared" si="0"/>
         <v>42339</v>
       </c>
@@ -8230,7 +8172,7 @@
       <c r="B62">
         <v>2016</v>
       </c>
-      <c r="C62" s="30">
+      <c r="C62" s="28">
         <f t="shared" si="0"/>
         <v>42370</v>
       </c>
@@ -8254,7 +8196,7 @@
       <c r="B63">
         <v>2016</v>
       </c>
-      <c r="C63" s="30">
+      <c r="C63" s="28">
         <f t="shared" si="0"/>
         <v>42401</v>
       </c>
@@ -8278,7 +8220,7 @@
       <c r="B64">
         <v>2016</v>
       </c>
-      <c r="C64" s="30">
+      <c r="C64" s="28">
         <f t="shared" si="0"/>
         <v>42430</v>
       </c>
@@ -8302,7 +8244,7 @@
       <c r="B65">
         <v>2016</v>
       </c>
-      <c r="C65" s="30">
+      <c r="C65" s="28">
         <f t="shared" si="0"/>
         <v>42461</v>
       </c>
@@ -8326,7 +8268,7 @@
       <c r="B66">
         <v>2016</v>
       </c>
-      <c r="C66" s="30">
+      <c r="C66" s="28">
         <f t="shared" si="0"/>
         <v>42491</v>
       </c>
@@ -8350,7 +8292,7 @@
       <c r="B67">
         <v>2016</v>
       </c>
-      <c r="C67" s="30">
+      <c r="C67" s="28">
         <f t="shared" ref="C67:C109" si="1">DATE(B67,A67,1)</f>
         <v>42522</v>
       </c>
@@ -8374,7 +8316,7 @@
       <c r="B68">
         <v>2016</v>
       </c>
-      <c r="C68" s="30">
+      <c r="C68" s="28">
         <f t="shared" si="1"/>
         <v>42552</v>
       </c>
@@ -8398,7 +8340,7 @@
       <c r="B69">
         <v>2016</v>
       </c>
-      <c r="C69" s="30">
+      <c r="C69" s="28">
         <f t="shared" si="1"/>
         <v>42583</v>
       </c>
@@ -8422,7 +8364,7 @@
       <c r="B70">
         <v>2016</v>
       </c>
-      <c r="C70" s="30">
+      <c r="C70" s="28">
         <f t="shared" si="1"/>
         <v>42614</v>
       </c>
@@ -8446,7 +8388,7 @@
       <c r="B71">
         <v>2016</v>
       </c>
-      <c r="C71" s="30">
+      <c r="C71" s="28">
         <f t="shared" si="1"/>
         <v>42644</v>
       </c>
@@ -8470,7 +8412,7 @@
       <c r="B72">
         <v>2016</v>
       </c>
-      <c r="C72" s="30">
+      <c r="C72" s="28">
         <f t="shared" si="1"/>
         <v>42675</v>
       </c>
@@ -8494,7 +8436,7 @@
       <c r="B73">
         <v>2016</v>
       </c>
-      <c r="C73" s="30">
+      <c r="C73" s="28">
         <f t="shared" si="1"/>
         <v>42705</v>
       </c>
@@ -8518,7 +8460,7 @@
       <c r="B74">
         <v>2017</v>
       </c>
-      <c r="C74" s="30">
+      <c r="C74" s="28">
         <f t="shared" si="1"/>
         <v>42736</v>
       </c>
@@ -8542,7 +8484,7 @@
       <c r="B75">
         <v>2017</v>
       </c>
-      <c r="C75" s="30">
+      <c r="C75" s="28">
         <f t="shared" si="1"/>
         <v>42767</v>
       </c>
@@ -8566,7 +8508,7 @@
       <c r="B76">
         <v>2017</v>
       </c>
-      <c r="C76" s="30">
+      <c r="C76" s="28">
         <f t="shared" si="1"/>
         <v>42795</v>
       </c>
@@ -8590,7 +8532,7 @@
       <c r="B77">
         <v>2017</v>
       </c>
-      <c r="C77" s="30">
+      <c r="C77" s="28">
         <f t="shared" si="1"/>
         <v>42826</v>
       </c>
@@ -8614,7 +8556,7 @@
       <c r="B78">
         <v>2017</v>
       </c>
-      <c r="C78" s="30">
+      <c r="C78" s="28">
         <f t="shared" si="1"/>
         <v>42856</v>
       </c>
@@ -8638,7 +8580,7 @@
       <c r="B79">
         <v>2017</v>
       </c>
-      <c r="C79" s="30">
+      <c r="C79" s="28">
         <f t="shared" si="1"/>
         <v>42887</v>
       </c>
@@ -8662,7 +8604,7 @@
       <c r="B80">
         <v>2017</v>
       </c>
-      <c r="C80" s="30">
+      <c r="C80" s="28">
         <f t="shared" si="1"/>
         <v>42917</v>
       </c>
@@ -8686,7 +8628,7 @@
       <c r="B81">
         <v>2017</v>
       </c>
-      <c r="C81" s="30">
+      <c r="C81" s="28">
         <f t="shared" si="1"/>
         <v>42948</v>
       </c>
@@ -8710,7 +8652,7 @@
       <c r="B82">
         <v>2017</v>
       </c>
-      <c r="C82" s="30">
+      <c r="C82" s="28">
         <f t="shared" si="1"/>
         <v>42979</v>
       </c>
@@ -8734,7 +8676,7 @@
       <c r="B83">
         <v>2017</v>
       </c>
-      <c r="C83" s="30">
+      <c r="C83" s="28">
         <f t="shared" si="1"/>
         <v>43009</v>
       </c>
@@ -8758,7 +8700,7 @@
       <c r="B84">
         <v>2017</v>
       </c>
-      <c r="C84" s="30">
+      <c r="C84" s="28">
         <f t="shared" si="1"/>
         <v>43040</v>
       </c>
@@ -8782,7 +8724,7 @@
       <c r="B85">
         <v>2017</v>
       </c>
-      <c r="C85" s="30">
+      <c r="C85" s="28">
         <f t="shared" si="1"/>
         <v>43070</v>
       </c>
@@ -8806,7 +8748,7 @@
       <c r="B86">
         <v>2018</v>
       </c>
-      <c r="C86" s="30">
+      <c r="C86" s="28">
         <f t="shared" si="1"/>
         <v>43101</v>
       </c>
@@ -8830,7 +8772,7 @@
       <c r="B87">
         <v>2018</v>
       </c>
-      <c r="C87" s="30">
+      <c r="C87" s="28">
         <f t="shared" si="1"/>
         <v>43132</v>
       </c>
@@ -8854,7 +8796,7 @@
       <c r="B88">
         <v>2018</v>
       </c>
-      <c r="C88" s="30">
+      <c r="C88" s="28">
         <f t="shared" si="1"/>
         <v>43160</v>
       </c>
@@ -8878,7 +8820,7 @@
       <c r="B89">
         <v>2018</v>
       </c>
-      <c r="C89" s="30">
+      <c r="C89" s="28">
         <f t="shared" si="1"/>
         <v>43191</v>
       </c>
@@ -8902,7 +8844,7 @@
       <c r="B90">
         <v>2018</v>
       </c>
-      <c r="C90" s="30">
+      <c r="C90" s="28">
         <f t="shared" si="1"/>
         <v>43221</v>
       </c>
@@ -8926,7 +8868,7 @@
       <c r="B91">
         <v>2018</v>
       </c>
-      <c r="C91" s="30">
+      <c r="C91" s="28">
         <f t="shared" si="1"/>
         <v>43252</v>
       </c>
@@ -8950,7 +8892,7 @@
       <c r="B92">
         <v>2018</v>
       </c>
-      <c r="C92" s="30">
+      <c r="C92" s="28">
         <f t="shared" si="1"/>
         <v>43282</v>
       </c>
@@ -8974,7 +8916,7 @@
       <c r="B93">
         <v>2018</v>
       </c>
-      <c r="C93" s="30">
+      <c r="C93" s="28">
         <f t="shared" si="1"/>
         <v>43313</v>
       </c>
@@ -8998,7 +8940,7 @@
       <c r="B94">
         <v>2018</v>
       </c>
-      <c r="C94" s="30">
+      <c r="C94" s="28">
         <f t="shared" si="1"/>
         <v>43344</v>
       </c>
@@ -9022,7 +8964,7 @@
       <c r="B95">
         <v>2018</v>
       </c>
-      <c r="C95" s="30">
+      <c r="C95" s="28">
         <f t="shared" si="1"/>
         <v>43374</v>
       </c>
@@ -9046,7 +8988,7 @@
       <c r="B96">
         <v>2018</v>
       </c>
-      <c r="C96" s="30">
+      <c r="C96" s="28">
         <f t="shared" si="1"/>
         <v>43405</v>
       </c>
@@ -9070,7 +9012,7 @@
       <c r="B97">
         <v>2018</v>
       </c>
-      <c r="C97" s="30">
+      <c r="C97" s="28">
         <f t="shared" si="1"/>
         <v>43435</v>
       </c>
@@ -9094,7 +9036,7 @@
       <c r="B98">
         <v>2019</v>
       </c>
-      <c r="C98" s="30">
+      <c r="C98" s="28">
         <f t="shared" si="1"/>
         <v>43466</v>
       </c>
@@ -9118,7 +9060,7 @@
       <c r="B99">
         <v>2019</v>
       </c>
-      <c r="C99" s="30">
+      <c r="C99" s="28">
         <f t="shared" si="1"/>
         <v>43497</v>
       </c>
@@ -9142,7 +9084,7 @@
       <c r="B100">
         <v>2019</v>
       </c>
-      <c r="C100" s="30">
+      <c r="C100" s="28">
         <f t="shared" si="1"/>
         <v>43525</v>
       </c>
@@ -9166,7 +9108,7 @@
       <c r="B101">
         <v>2019</v>
       </c>
-      <c r="C101" s="30">
+      <c r="C101" s="28">
         <f t="shared" si="1"/>
         <v>43556</v>
       </c>
@@ -9190,7 +9132,7 @@
       <c r="B102">
         <v>2019</v>
       </c>
-      <c r="C102" s="30">
+      <c r="C102" s="28">
         <f t="shared" si="1"/>
         <v>43586</v>
       </c>
@@ -9214,7 +9156,7 @@
       <c r="B103">
         <v>2019</v>
       </c>
-      <c r="C103" s="30">
+      <c r="C103" s="28">
         <f t="shared" si="1"/>
         <v>43617</v>
       </c>
@@ -9238,7 +9180,7 @@
       <c r="B104">
         <v>2019</v>
       </c>
-      <c r="C104" s="30">
+      <c r="C104" s="28">
         <f t="shared" si="1"/>
         <v>43647</v>
       </c>
@@ -9262,7 +9204,7 @@
       <c r="B105">
         <v>2019</v>
       </c>
-      <c r="C105" s="30">
+      <c r="C105" s="28">
         <f t="shared" si="1"/>
         <v>43678</v>
       </c>
@@ -9286,7 +9228,7 @@
       <c r="B106">
         <v>2019</v>
       </c>
-      <c r="C106" s="30">
+      <c r="C106" s="28">
         <f t="shared" si="1"/>
         <v>43709</v>
       </c>
@@ -9310,7 +9252,7 @@
       <c r="B107">
         <v>2019</v>
       </c>
-      <c r="C107" s="30">
+      <c r="C107" s="28">
         <f t="shared" si="1"/>
         <v>43739</v>
       </c>
@@ -9334,7 +9276,7 @@
       <c r="B108">
         <v>2019</v>
       </c>
-      <c r="C108" s="30">
+      <c r="C108" s="28">
         <f t="shared" si="1"/>
         <v>43770</v>
       </c>
@@ -9358,7 +9300,7 @@
       <c r="B109">
         <v>2019</v>
       </c>
-      <c r="C109" s="30">
+      <c r="C109" s="28">
         <f t="shared" si="1"/>
         <v>43800</v>
       </c>

</xml_diff>